<commit_message>
#1 Updated ASVS checklist
</commit_message>
<xml_diff>
--- a/Deliverables/Documentation/P2/v4-ASVS-checklist-en_sprint_1.xlsx
+++ b/Deliverables/Documentation/P2/v4-ASVS-checklist-en_sprint_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ISEP\repos\desofs2024_M1A_1\Deliverables\diagrams\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/49d711c5891ea100/Documentos/GitHub/desofs2024_M1A_1/Deliverables/Documentation/P2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C78AB6-E857-4C84-8D3C-E9F51CD278B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="13_ncr:1_{B8C78AB6-E857-4C84-8D3C-E9F51CD278B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6BF7A1E-E827-4312-A435-8E7750A1BB0B}"/>
   <bookViews>
-    <workbookView xWindow="41295" yWindow="-5325" windowWidth="25905" windowHeight="21000" tabRatio="831" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="831" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASVS Results" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="695">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="711">
   <si>
     <t>Security Category</t>
   </si>
@@ -2171,6 +2171,54 @@
   <si>
     <t>Non-valid</t>
   </si>
+  <si>
+    <t>pt.isep.desofs.m1a.g1.config.InputSanitizer</t>
+  </si>
+  <si>
+    <t>Input validation and sanitization are implemented to protect against injection attacks. The InputSanitizer class is used to sanitize inputs and ensure they do not contain malicious content.</t>
+  </si>
+  <si>
+    <t>Manual code review and OWASP ZAP</t>
+  </si>
+  <si>
+    <t>pt.isep.desofs.m1a.g1.controller.GlobalExceptionHandler</t>
+  </si>
+  <si>
+    <t>All input validation failures result in input rejection. The GlobalExceptionHandler class handles validation exceptions and returns appropriate HTTP response statuses.</t>
+  </si>
+  <si>
+    <t>Manual code review and Postman</t>
+  </si>
+  <si>
+    <t>Input sanitization is implemented to filter or reject unexpected characters. The InputSanitizer class sanitizes inputs to eliminate any characters that could lead to injection attacks.</t>
+  </si>
+  <si>
+    <t>Input validation errors are handled securely using the GlobalExceptionHandler class. Errors are logged appropriately, and generic error messages are returned to the user without exposing sensitive information.</t>
+  </si>
+  <si>
+    <t>pt.isep.desofs.m1a.g1.config.InputValidator</t>
+  </si>
+  <si>
+    <t>A centralized input validation mechanism is implemented in the InputValidator class. This class provides validation methods that can be accessed and used by all components of the application to ensure consistent input validation.</t>
+  </si>
+  <si>
+    <t>The InputSanitizer class ensures that all inputs are validated using positive validation.</t>
+  </si>
+  <si>
+    <t>The InputSanitizer class sanitizes unstructured text fields to remove harmful content.</t>
+  </si>
+  <si>
+    <t>The InputSanitizer class includes mechanisms for validating and sanitizing file uploads.</t>
+  </si>
+  <si>
+    <t>Input validation errors are handled securely using GlobalExceptionHandler. The InputSanitizer ensures inputs are sanitized before processing.</t>
+  </si>
+  <si>
+    <t>Context-aware output encoding and escaping are applied using InputSanitizer.</t>
+  </si>
+  <si>
+    <t>The GlobalExceptionHandler class ensures that a generic message is shown when an unexpected or security-sensitive error occurs. It generates a unique ID for each error, which can be used by support personnel for investigation.</t>
+  </si>
 </sst>
 </file>
 
@@ -2179,7 +2227,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00,_€;\-#,##0.00,_€"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2265,6 +2313,14 @@
       <sz val="12"/>
       <color rgb="FF102A43"/>
       <name val="Noto Sans CJK SC"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF102A43"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -2941,7 +2997,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3185,7 +3241,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3260,6 +3315,22 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3532,13 +3603,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>33.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>8.3333333333333321</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -3562,7 +3633,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.0359712230215825</c:v>
+                  <c:v>8.9928057553956826</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4077,21 +4148,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="64.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="64.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="21" style="4" customWidth="1"/>
     <col min="4" max="4" width="25" style="4" customWidth="1"/>
     <col min="5" max="5" width="37" style="4" customWidth="1"/>
-    <col min="6" max="1024" width="8.85546875" style="4"/>
+    <col min="6" max="1024" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="7" customFormat="1" ht="42">
+    <row r="1" spans="1:6" s="7" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4186,7 +4257,7 @@
       </c>
       <c r="B6" s="9">
         <f>COUNTIF('Validation, Sanitization and En'!G2:G31,"Valid")</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C6" s="10">
         <f>COUNTIF('Validation, Sanitization and En'!G2:G31,"&lt;&gt;Not Applicable")</f>
@@ -4194,7 +4265,7 @@
       </c>
       <c r="D6" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>33.333333333333329</v>
       </c>
       <c r="E6" s="12"/>
     </row>
@@ -4223,7 +4294,7 @@
       </c>
       <c r="B8" s="9">
         <f>COUNTIF('Error Handling and Logging'!G2:G14,"Valid")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="10">
         <f>COUNTIF('Error Handling and Logging'!G2:G14,"&lt;&gt;Not Applicable")</f>
@@ -4231,7 +4302,7 @@
       </c>
       <c r="D8" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3333333333333321</v>
       </c>
       <c r="E8" s="12"/>
     </row>
@@ -4367,7 +4438,7 @@
       </c>
       <c r="B16" s="9">
         <f>SUM(B2:B15)</f>
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C16" s="10">
         <f>SUM(C2:C15)</f>
@@ -4375,7 +4446,7 @@
       </c>
       <c r="D16" s="11">
         <f t="shared" si="0"/>
-        <v>5.0359712230215825</v>
+        <v>8.9928057553956826</v>
       </c>
       <c r="E16" s="12"/>
     </row>
@@ -4398,21 +4469,21 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" style="72" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="25"/>
-    <col min="3" max="5" width="8.85546875" style="59"/>
-    <col min="6" max="6" width="88.85546875" style="25" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="25"/>
-    <col min="8" max="8" width="28.28515625" style="25" customWidth="1"/>
-    <col min="9" max="9" width="26.28515625" style="25" customWidth="1"/>
-    <col min="10" max="10" width="37.7109375" style="25" customWidth="1"/>
-    <col min="11" max="1024" width="8.85546875" style="25"/>
+    <col min="1" max="1" width="37.33203125" style="72" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="25"/>
+    <col min="3" max="5" width="8.88671875" style="59"/>
+    <col min="6" max="6" width="88.88671875" style="25" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="25"/>
+    <col min="8" max="8" width="28.33203125" style="25" customWidth="1"/>
+    <col min="9" max="9" width="26.33203125" style="25" customWidth="1"/>
+    <col min="10" max="10" width="37.6640625" style="25" customWidth="1"/>
+    <col min="11" max="1024" width="8.88671875" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="43" customFormat="1" ht="42">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="93" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="61" t="s">
@@ -4444,7 +4515,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="48" customHeight="1">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="120" t="s">
         <v>505</v>
       </c>
       <c r="B2" s="62" t="s">
@@ -4465,8 +4536,8 @@
       <c r="I2" s="49"/>
       <c r="J2" s="65"/>
     </row>
-    <row r="3" spans="1:10" ht="31.5">
-      <c r="A3" s="121"/>
+    <row r="3" spans="1:10" ht="31.2">
+      <c r="A3" s="120"/>
       <c r="B3" s="62" t="s">
         <v>508</v>
       </c>
@@ -4485,8 +4556,8 @@
       <c r="I3" s="28"/>
       <c r="J3" s="32"/>
     </row>
-    <row r="4" spans="1:10" ht="31.5">
-      <c r="A4" s="121"/>
+    <row r="4" spans="1:10" ht="31.2">
+      <c r="A4" s="120"/>
       <c r="B4" s="62" t="s">
         <v>510</v>
       </c>
@@ -4506,7 +4577,7 @@
       <c r="J4" s="32"/>
     </row>
     <row r="5" spans="1:10" ht="63.75" customHeight="1">
-      <c r="A5" s="121" t="s">
+      <c r="A5" s="120" t="s">
         <v>512</v>
       </c>
       <c r="B5" s="62" t="s">
@@ -4527,8 +4598,8 @@
       <c r="I5" s="28"/>
       <c r="J5" s="32"/>
     </row>
-    <row r="6" spans="1:10" ht="63">
-      <c r="A6" s="121"/>
+    <row r="6" spans="1:10" ht="62.4">
+      <c r="A6" s="120"/>
       <c r="B6" s="62" t="s">
         <v>515</v>
       </c>
@@ -4547,8 +4618,8 @@
       <c r="I6" s="28"/>
       <c r="J6" s="32"/>
     </row>
-    <row r="7" spans="1:10" ht="31.5">
-      <c r="A7" s="121"/>
+    <row r="7" spans="1:10" ht="31.2">
+      <c r="A7" s="120"/>
       <c r="B7" s="62" t="s">
         <v>517</v>
       </c>
@@ -4567,8 +4638,8 @@
       <c r="I7" s="28"/>
       <c r="J7" s="32"/>
     </row>
-    <row r="8" spans="1:10" ht="31.5">
-      <c r="A8" s="121"/>
+    <row r="8" spans="1:10" ht="31.2">
+      <c r="A8" s="120"/>
       <c r="B8" s="62" t="s">
         <v>519</v>
       </c>
@@ -4587,12 +4658,12 @@
       <c r="I8" s="28"/>
       <c r="J8" s="32"/>
     </row>
-    <row r="9" spans="1:10" ht="15.75">
-      <c r="A9" s="121"/>
+    <row r="9" spans="1:10" ht="15.6">
+      <c r="A9" s="120"/>
       <c r="B9" s="62" t="s">
         <v>521</v>
       </c>
-      <c r="C9" s="95">
+      <c r="C9" s="94">
         <v>3</v>
       </c>
       <c r="D9" s="34">
@@ -4635,21 +4706,21 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" style="72" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="25"/>
-    <col min="3" max="5" width="8.85546875" style="59"/>
-    <col min="6" max="6" width="88.42578125" style="25" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="25"/>
-    <col min="8" max="8" width="35.85546875" style="25" customWidth="1"/>
-    <col min="9" max="9" width="26.140625" style="25" customWidth="1"/>
-    <col min="10" max="10" width="28.7109375" style="25" customWidth="1"/>
-    <col min="11" max="1024" width="8.85546875" style="25"/>
+    <col min="1" max="1" width="31.44140625" style="72" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="25"/>
+    <col min="3" max="5" width="8.88671875" style="59"/>
+    <col min="6" max="6" width="88.44140625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="25"/>
+    <col min="8" max="8" width="35.88671875" style="25" customWidth="1"/>
+    <col min="9" max="9" width="26.109375" style="25" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" style="25" customWidth="1"/>
+    <col min="11" max="1024" width="8.88671875" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="43" customFormat="1" ht="42">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="95" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="61" t="s">
@@ -4680,14 +4751,14 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="31.5">
+    <row r="2" spans="1:10" ht="31.2">
       <c r="A2" s="1" t="s">
         <v>523</v>
       </c>
       <c r="B2" s="62" t="s">
         <v>524</v>
       </c>
-      <c r="C2" s="97">
+      <c r="C2" s="96">
         <v>3</v>
       </c>
       <c r="D2" s="47">
@@ -4703,7 +4774,7 @@
       <c r="J2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="48" customHeight="1">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="120" t="s">
         <v>526</v>
       </c>
       <c r="B3" s="62" t="s">
@@ -4724,8 +4795,8 @@
       <c r="I3" s="28"/>
       <c r="J3" s="32"/>
     </row>
-    <row r="4" spans="1:10" ht="31.5">
-      <c r="A4" s="121"/>
+    <row r="4" spans="1:10" ht="31.2">
+      <c r="A4" s="120"/>
       <c r="B4" s="62" t="s">
         <v>529</v>
       </c>
@@ -4744,8 +4815,8 @@
       <c r="I4" s="28"/>
       <c r="J4" s="32"/>
     </row>
-    <row r="5" spans="1:10" ht="78.75">
-      <c r="A5" s="121"/>
+    <row r="5" spans="1:10" ht="78">
+      <c r="A5" s="120"/>
       <c r="B5" s="62" t="s">
         <v>531</v>
       </c>
@@ -4764,8 +4835,8 @@
       <c r="I5" s="28"/>
       <c r="J5" s="32"/>
     </row>
-    <row r="6" spans="1:10" ht="31.5">
-      <c r="A6" s="121"/>
+    <row r="6" spans="1:10" ht="31.2">
+      <c r="A6" s="120"/>
       <c r="B6" s="62" t="s">
         <v>533</v>
       </c>
@@ -4784,8 +4855,8 @@
       <c r="I6" s="28"/>
       <c r="J6" s="32"/>
     </row>
-    <row r="7" spans="1:10" ht="31.5">
-      <c r="A7" s="121"/>
+    <row r="7" spans="1:10" ht="31.2">
+      <c r="A7" s="120"/>
       <c r="B7" s="62" t="s">
         <v>535</v>
       </c>
@@ -4804,8 +4875,8 @@
       <c r="I7" s="28"/>
       <c r="J7" s="32"/>
     </row>
-    <row r="8" spans="1:10" ht="31.5">
-      <c r="A8" s="121"/>
+    <row r="8" spans="1:10" ht="31.2">
+      <c r="A8" s="120"/>
       <c r="B8" s="62" t="s">
         <v>537</v>
       </c>
@@ -4825,7 +4896,7 @@
       <c r="J8" s="32"/>
     </row>
     <row r="9" spans="1:10" ht="48" customHeight="1">
-      <c r="A9" s="121" t="s">
+      <c r="A9" s="120" t="s">
         <v>539</v>
       </c>
       <c r="B9" s="62" t="s">
@@ -4846,8 +4917,8 @@
       <c r="I9" s="28"/>
       <c r="J9" s="32"/>
     </row>
-    <row r="10" spans="1:10" ht="63">
-      <c r="A10" s="121"/>
+    <row r="10" spans="1:10" ht="62.4">
+      <c r="A10" s="120"/>
       <c r="B10" s="62" t="s">
         <v>542</v>
       </c>
@@ -4866,8 +4937,8 @@
       <c r="I10" s="28"/>
       <c r="J10" s="32"/>
     </row>
-    <row r="11" spans="1:10" ht="94.5">
-      <c r="A11" s="121"/>
+    <row r="11" spans="1:10" ht="93.6">
+      <c r="A11" s="120"/>
       <c r="B11" s="62" t="s">
         <v>544</v>
       </c>
@@ -4914,21 +4985,21 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="72" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="25"/>
-    <col min="3" max="5" width="8.85546875" style="59"/>
-    <col min="6" max="6" width="71.28515625" style="25" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="25" customWidth="1"/>
-    <col min="8" max="8" width="34.7109375" style="25" customWidth="1"/>
-    <col min="9" max="9" width="34.42578125" style="25" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="72" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="25"/>
+    <col min="3" max="5" width="8.88671875" style="59"/>
+    <col min="6" max="6" width="71.33203125" style="25" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" style="25" customWidth="1"/>
+    <col min="8" max="8" width="34.6640625" style="25" customWidth="1"/>
+    <col min="9" max="9" width="34.44140625" style="25" customWidth="1"/>
     <col min="10" max="10" width="37" style="25" customWidth="1"/>
-    <col min="11" max="1024" width="8.85546875" style="25"/>
+    <col min="11" max="1024" width="8.88671875" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="43" customFormat="1" ht="42">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="93" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="61" t="s">
@@ -4960,7 +5031,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="120" t="s">
         <v>546</v>
       </c>
       <c r="B2" s="62" t="s">
@@ -4981,8 +5052,8 @@
       <c r="I2" s="49"/>
       <c r="J2" s="65"/>
     </row>
-    <row r="3" spans="1:10" ht="47.25">
-      <c r="A3" s="121"/>
+    <row r="3" spans="1:10" ht="46.8">
+      <c r="A3" s="120"/>
       <c r="B3" s="62" t="s">
         <v>549</v>
       </c>
@@ -5001,8 +5072,8 @@
       <c r="I3" s="28"/>
       <c r="J3" s="32"/>
     </row>
-    <row r="4" spans="1:10" ht="31.5">
-      <c r="A4" s="121"/>
+    <row r="4" spans="1:10" ht="31.2">
+      <c r="A4" s="120"/>
       <c r="B4" s="62" t="s">
         <v>551</v>
       </c>
@@ -5021,8 +5092,8 @@
       <c r="I4" s="28"/>
       <c r="J4" s="32"/>
     </row>
-    <row r="5" spans="1:10" ht="47.25">
-      <c r="A5" s="121"/>
+    <row r="5" spans="1:10" ht="46.8">
+      <c r="A5" s="120"/>
       <c r="B5" s="62" t="s">
         <v>553</v>
       </c>
@@ -5041,8 +5112,8 @@
       <c r="I5" s="28"/>
       <c r="J5" s="32"/>
     </row>
-    <row r="6" spans="1:10" ht="47.25">
-      <c r="A6" s="121"/>
+    <row r="6" spans="1:10" ht="46.8">
+      <c r="A6" s="120"/>
       <c r="B6" s="62" t="s">
         <v>555</v>
       </c>
@@ -5062,7 +5133,7 @@
       <c r="J6" s="32"/>
     </row>
     <row r="7" spans="1:10" ht="36" customHeight="1">
-      <c r="A7" s="121"/>
+      <c r="A7" s="120"/>
       <c r="B7" s="62" t="s">
         <v>557</v>
       </c>
@@ -5082,7 +5153,7 @@
       <c r="J7" s="32"/>
     </row>
     <row r="8" spans="1:10" ht="66.75" customHeight="1">
-      <c r="A8" s="121"/>
+      <c r="A8" s="120"/>
       <c r="B8" s="62" t="s">
         <v>559</v>
       </c>
@@ -5101,8 +5172,8 @@
       <c r="I8" s="28"/>
       <c r="J8" s="32"/>
     </row>
-    <row r="9" spans="1:10" ht="31.5">
-      <c r="A9" s="121"/>
+    <row r="9" spans="1:10" ht="31.2">
+      <c r="A9" s="120"/>
       <c r="B9" s="62" t="s">
         <v>561</v>
       </c>
@@ -5148,21 +5219,21 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" style="72" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="25" customWidth="1"/>
-    <col min="3" max="5" width="8.85546875" style="59"/>
-    <col min="6" max="6" width="78.7109375" style="25" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" style="25" customWidth="1"/>
-    <col min="8" max="8" width="31.42578125" style="25" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" style="25" customWidth="1"/>
-    <col min="10" max="10" width="31.85546875" style="25" customWidth="1"/>
-    <col min="11" max="1024" width="8.85546875" style="25"/>
+    <col min="1" max="1" width="33.5546875" style="72" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="25" customWidth="1"/>
+    <col min="3" max="5" width="8.88671875" style="59"/>
+    <col min="6" max="6" width="78.6640625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" style="25" customWidth="1"/>
+    <col min="8" max="8" width="31.44140625" style="25" customWidth="1"/>
+    <col min="9" max="9" width="26.88671875" style="25" customWidth="1"/>
+    <col min="10" max="10" width="31.88671875" style="25" customWidth="1"/>
+    <col min="11" max="1024" width="8.88671875" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="43" customFormat="1" ht="42">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="93" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="61" t="s">
@@ -5194,7 +5265,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="120" t="s">
         <v>563</v>
       </c>
       <c r="B2" s="62" t="s">
@@ -5215,8 +5286,8 @@
       <c r="I2" s="49"/>
       <c r="J2" s="65"/>
     </row>
-    <row r="3" spans="1:10" ht="47.25">
-      <c r="A3" s="121"/>
+    <row r="3" spans="1:10" ht="46.8">
+      <c r="A3" s="120"/>
       <c r="B3" s="62" t="s">
         <v>566</v>
       </c>
@@ -5235,8 +5306,8 @@
       <c r="I3" s="28"/>
       <c r="J3" s="32"/>
     </row>
-    <row r="4" spans="1:10" ht="47.25">
-      <c r="A4" s="121"/>
+    <row r="4" spans="1:10" ht="46.8">
+      <c r="A4" s="120"/>
       <c r="B4" s="62" t="s">
         <v>568</v>
       </c>
@@ -5255,7 +5326,7 @@
       <c r="I4" s="28"/>
       <c r="J4" s="32"/>
     </row>
-    <row r="5" spans="1:10" ht="31.5">
+    <row r="5" spans="1:10" ht="31.2">
       <c r="A5" s="1" t="s">
         <v>570</v>
       </c>
@@ -5278,7 +5349,7 @@
       <c r="J5" s="32"/>
     </row>
     <row r="6" spans="1:10" ht="48" customHeight="1">
-      <c r="A6" s="121" t="s">
+      <c r="A6" s="120" t="s">
         <v>573</v>
       </c>
       <c r="B6" s="62" t="s">
@@ -5299,8 +5370,8 @@
       <c r="I6" s="28"/>
       <c r="J6" s="32"/>
     </row>
-    <row r="7" spans="1:10" ht="31.5">
-      <c r="A7" s="121"/>
+    <row r="7" spans="1:10" ht="31.2">
+      <c r="A7" s="120"/>
       <c r="B7" s="62" t="s">
         <v>576</v>
       </c>
@@ -5319,8 +5390,8 @@
       <c r="I7" s="28"/>
       <c r="J7" s="32"/>
     </row>
-    <row r="8" spans="1:10" ht="47.25">
-      <c r="A8" s="121"/>
+    <row r="8" spans="1:10" ht="46.8">
+      <c r="A8" s="120"/>
       <c r="B8" s="62" t="s">
         <v>578</v>
       </c>
@@ -5339,8 +5410,8 @@
       <c r="I8" s="28"/>
       <c r="J8" s="32"/>
     </row>
-    <row r="9" spans="1:10" ht="63">
-      <c r="A9" s="121"/>
+    <row r="9" spans="1:10" ht="62.4">
+      <c r="A9" s="120"/>
       <c r="B9" s="62" t="s">
         <v>580</v>
       </c>
@@ -5359,8 +5430,8 @@
       <c r="I9" s="28"/>
       <c r="J9" s="32"/>
     </row>
-    <row r="10" spans="1:10" ht="31.5">
-      <c r="A10" s="121"/>
+    <row r="10" spans="1:10" ht="31.2">
+      <c r="A10" s="120"/>
       <c r="B10" s="62" t="s">
         <v>582</v>
       </c>
@@ -5379,8 +5450,8 @@
       <c r="I10" s="28"/>
       <c r="J10" s="32"/>
     </row>
-    <row r="11" spans="1:10" ht="47.25">
-      <c r="A11" s="121"/>
+    <row r="11" spans="1:10" ht="46.8">
+      <c r="A11" s="120"/>
       <c r="B11" s="62" t="s">
         <v>584</v>
       </c>
@@ -5400,7 +5471,7 @@
       <c r="J11" s="32"/>
     </row>
     <row r="12" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A12" s="121" t="s">
+      <c r="A12" s="120" t="s">
         <v>586</v>
       </c>
       <c r="B12" s="62" t="s">
@@ -5421,8 +5492,8 @@
       <c r="I12" s="28"/>
       <c r="J12" s="32"/>
     </row>
-    <row r="13" spans="1:10" ht="31.5">
-      <c r="A13" s="121"/>
+    <row r="13" spans="1:10" ht="31.2">
+      <c r="A13" s="120"/>
       <c r="B13" s="62" t="s">
         <v>589</v>
       </c>
@@ -5442,7 +5513,7 @@
       <c r="J13" s="32"/>
     </row>
     <row r="14" spans="1:10" ht="79.5" customHeight="1">
-      <c r="A14" s="121" t="s">
+      <c r="A14" s="120" t="s">
         <v>591</v>
       </c>
       <c r="B14" s="62" t="s">
@@ -5463,8 +5534,8 @@
       <c r="I14" s="28"/>
       <c r="J14" s="32"/>
     </row>
-    <row r="15" spans="1:10" ht="31.5">
-      <c r="A15" s="121"/>
+    <row r="15" spans="1:10" ht="31.2">
+      <c r="A15" s="120"/>
       <c r="B15" s="62" t="s">
         <v>594</v>
       </c>
@@ -5483,7 +5554,7 @@
       <c r="I15" s="28"/>
       <c r="J15" s="32"/>
     </row>
-    <row r="16" spans="1:10" ht="47.25">
+    <row r="16" spans="1:10" ht="46.8">
       <c r="A16" s="1" t="s">
         <v>596</v>
       </c>
@@ -5535,20 +5606,20 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21"/>
   <cols>
     <col min="1" max="1" width="24" style="72" customWidth="1"/>
-    <col min="2" max="5" width="8.85546875" style="25"/>
-    <col min="6" max="6" width="84.42578125" style="25" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" style="25" customWidth="1"/>
-    <col min="8" max="8" width="35.42578125" style="25" customWidth="1"/>
-    <col min="9" max="9" width="24.140625" style="25" customWidth="1"/>
-    <col min="10" max="10" width="37.85546875" style="25" customWidth="1"/>
-    <col min="11" max="1024" width="8.85546875" style="25"/>
+    <col min="2" max="5" width="8.88671875" style="25"/>
+    <col min="6" max="6" width="84.44140625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="17.5546875" style="25" customWidth="1"/>
+    <col min="8" max="8" width="35.44140625" style="25" customWidth="1"/>
+    <col min="9" max="9" width="24.109375" style="25" customWidth="1"/>
+    <col min="10" max="10" width="37.88671875" style="25" customWidth="1"/>
+    <col min="11" max="1024" width="8.88671875" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="43" customFormat="1" ht="42">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="93" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="61" t="s">
@@ -5580,7 +5651,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="48" customHeight="1">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="120" t="s">
         <v>599</v>
       </c>
       <c r="B2" s="62" t="s">
@@ -5601,8 +5672,8 @@
       <c r="I2" s="49"/>
       <c r="J2" s="65"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75">
-      <c r="A3" s="121"/>
+    <row r="3" spans="1:10" ht="15.6">
+      <c r="A3" s="120"/>
       <c r="B3" s="62" t="s">
         <v>602</v>
       </c>
@@ -5623,8 +5694,8 @@
       <c r="I3" s="28"/>
       <c r="J3" s="32"/>
     </row>
-    <row r="4" spans="1:10" ht="31.5">
-      <c r="A4" s="121"/>
+    <row r="4" spans="1:10" ht="31.2">
+      <c r="A4" s="120"/>
       <c r="B4" s="62" t="s">
         <v>604</v>
       </c>
@@ -5643,8 +5714,8 @@
       <c r="I4" s="28"/>
       <c r="J4" s="32"/>
     </row>
-    <row r="5" spans="1:10" ht="47.25">
-      <c r="A5" s="121"/>
+    <row r="5" spans="1:10" ht="46.8">
+      <c r="A5" s="120"/>
       <c r="B5" s="62" t="s">
         <v>606</v>
       </c>
@@ -5663,8 +5734,8 @@
       <c r="I5" s="28"/>
       <c r="J5" s="32"/>
     </row>
-    <row r="6" spans="1:10" ht="47.25">
-      <c r="A6" s="121"/>
+    <row r="6" spans="1:10" ht="46.8">
+      <c r="A6" s="120"/>
       <c r="B6" s="62" t="s">
         <v>608</v>
       </c>
@@ -5684,7 +5755,7 @@
       <c r="J6" s="32"/>
     </row>
     <row r="7" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A7" s="121" t="s">
+      <c r="A7" s="120" t="s">
         <v>610</v>
       </c>
       <c r="B7" s="62" t="s">
@@ -5705,8 +5776,8 @@
       <c r="I7" s="28"/>
       <c r="J7" s="32"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75">
-      <c r="A8" s="121"/>
+    <row r="8" spans="1:10" ht="15.6">
+      <c r="A8" s="120"/>
       <c r="B8" s="62" t="s">
         <v>613</v>
       </c>
@@ -5725,8 +5796,8 @@
       <c r="I8" s="28"/>
       <c r="J8" s="32"/>
     </row>
-    <row r="9" spans="1:10" ht="47.25">
-      <c r="A9" s="121"/>
+    <row r="9" spans="1:10" ht="46.8">
+      <c r="A9" s="120"/>
       <c r="B9" s="62" t="s">
         <v>615</v>
       </c>
@@ -5745,8 +5816,8 @@
       <c r="I9" s="28"/>
       <c r="J9" s="32"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75">
-      <c r="A10" s="121"/>
+    <row r="10" spans="1:10" ht="15.6">
+      <c r="A10" s="120"/>
       <c r="B10" s="62" t="s">
         <v>617</v>
       </c>
@@ -5767,8 +5838,8 @@
       <c r="I10" s="28"/>
       <c r="J10" s="32"/>
     </row>
-    <row r="11" spans="1:10" ht="31.5">
-      <c r="A11" s="121"/>
+    <row r="11" spans="1:10" ht="31.2">
+      <c r="A11" s="120"/>
       <c r="B11" s="62" t="s">
         <v>619</v>
       </c>
@@ -5787,8 +5858,8 @@
       <c r="I11" s="28"/>
       <c r="J11" s="32"/>
     </row>
-    <row r="12" spans="1:10" ht="94.5">
-      <c r="A12" s="121"/>
+    <row r="12" spans="1:10" ht="93.6">
+      <c r="A12" s="120"/>
       <c r="B12" s="62" t="s">
         <v>621</v>
       </c>
@@ -5808,7 +5879,7 @@
       <c r="J12" s="32"/>
     </row>
     <row r="13" spans="1:10" ht="48" customHeight="1">
-      <c r="A13" s="121" t="s">
+      <c r="A13" s="120" t="s">
         <v>623</v>
       </c>
       <c r="B13" s="62" t="s">
@@ -5829,8 +5900,8 @@
       <c r="I13" s="28"/>
       <c r="J13" s="32"/>
     </row>
-    <row r="14" spans="1:10" ht="31.5">
-      <c r="A14" s="121"/>
+    <row r="14" spans="1:10" ht="31.2">
+      <c r="A14" s="120"/>
       <c r="B14" s="62" t="s">
         <v>626</v>
       </c>
@@ -5850,7 +5921,7 @@
       <c r="J14" s="32"/>
     </row>
     <row r="15" spans="1:10" ht="63.75" customHeight="1">
-      <c r="A15" s="121" t="s">
+      <c r="A15" s="120" t="s">
         <v>628</v>
       </c>
       <c r="B15" s="62" t="s">
@@ -5871,8 +5942,8 @@
       <c r="I15" s="28"/>
       <c r="J15" s="32"/>
     </row>
-    <row r="16" spans="1:10" ht="31.5">
-      <c r="A16" s="121"/>
+    <row r="16" spans="1:10" ht="31.2">
+      <c r="A16" s="120"/>
       <c r="B16" s="62" t="s">
         <v>631</v>
       </c>
@@ -5921,21 +5992,21 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" style="72" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="25" customWidth="1"/>
-    <col min="3" max="5" width="8.85546875" style="25"/>
-    <col min="6" max="6" width="88.7109375" style="25" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" style="25" customWidth="1"/>
-    <col min="8" max="8" width="35.28515625" style="25" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" style="25" customWidth="1"/>
-    <col min="10" max="10" width="33.42578125" style="25" customWidth="1"/>
-    <col min="11" max="1024" width="8.85546875" style="25"/>
+    <col min="1" max="1" width="40.88671875" style="72" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="25" customWidth="1"/>
+    <col min="3" max="5" width="8.88671875" style="25"/>
+    <col min="6" max="6" width="88.6640625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="17.109375" style="25" customWidth="1"/>
+    <col min="8" max="8" width="35.33203125" style="25" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" style="25" customWidth="1"/>
+    <col min="10" max="10" width="33.44140625" style="25" customWidth="1"/>
+    <col min="11" max="1024" width="8.88671875" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="43" customFormat="1" ht="42">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="97" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="86" t="s">
@@ -5967,508 +6038,508 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="48" customHeight="1">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="121" t="s">
         <v>633</v>
       </c>
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="98" t="s">
         <v>634</v>
       </c>
-      <c r="C2" s="100">
-        <v>2</v>
-      </c>
-      <c r="D2" s="101"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="103" t="s">
+      <c r="C2" s="99">
+        <v>2</v>
+      </c>
+      <c r="D2" s="100"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="102" t="s">
         <v>635</v>
       </c>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
-      <c r="I2" s="104"/>
-      <c r="J2" s="105"/>
-    </row>
-    <row r="3" spans="1:10" ht="47.25">
-      <c r="A3" s="122"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="104"/>
+    </row>
+    <row r="3" spans="1:10" ht="46.8">
+      <c r="A3" s="121"/>
       <c r="B3" s="62" t="s">
         <v>636</v>
       </c>
-      <c r="C3" s="106">
-        <v>2</v>
-      </c>
-      <c r="D3" s="107">
+      <c r="C3" s="105">
+        <v>2</v>
+      </c>
+      <c r="D3" s="106">
         <v>120</v>
       </c>
-      <c r="E3" s="108"/>
-      <c r="F3" s="109" t="s">
+      <c r="E3" s="107"/>
+      <c r="F3" s="108" t="s">
         <v>637</v>
       </c>
-      <c r="G3" s="110"/>
-      <c r="H3" s="110"/>
-      <c r="I3" s="110"/>
-      <c r="J3" s="111"/>
-    </row>
-    <row r="4" spans="1:10" ht="31.5">
-      <c r="A4" s="122"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="110"/>
+    </row>
+    <row r="4" spans="1:10" ht="31.2">
+      <c r="A4" s="121"/>
       <c r="B4" s="62" t="s">
         <v>638</v>
       </c>
-      <c r="C4" s="106">
-        <v>2</v>
-      </c>
-      <c r="D4" s="107">
+      <c r="C4" s="105">
+        <v>2</v>
+      </c>
+      <c r="D4" s="106">
         <v>16</v>
       </c>
-      <c r="E4" s="108"/>
-      <c r="F4" s="109" t="s">
+      <c r="E4" s="107"/>
+      <c r="F4" s="108" t="s">
         <v>639</v>
       </c>
-      <c r="G4" s="110"/>
-      <c r="H4" s="110"/>
-      <c r="I4" s="110"/>
-      <c r="J4" s="111"/>
-    </row>
-    <row r="5" spans="1:10" ht="47.25">
-      <c r="A5" s="122"/>
+      <c r="G4" s="109"/>
+      <c r="H4" s="109"/>
+      <c r="I4" s="109"/>
+      <c r="J4" s="110"/>
+    </row>
+    <row r="5" spans="1:10" ht="46.8">
+      <c r="A5" s="121"/>
       <c r="B5" s="62" t="s">
         <v>640</v>
       </c>
-      <c r="C5" s="106">
-        <v>2</v>
-      </c>
-      <c r="D5" s="107"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="109" t="s">
+      <c r="C5" s="105">
+        <v>2</v>
+      </c>
+      <c r="D5" s="106"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="108" t="s">
         <v>641</v>
       </c>
-      <c r="G5" s="110"/>
-      <c r="H5" s="110"/>
-      <c r="I5" s="110"/>
-      <c r="J5" s="111"/>
-    </row>
-    <row r="6" spans="1:10" ht="31.5">
-      <c r="A6" s="122"/>
+      <c r="G5" s="109"/>
+      <c r="H5" s="109"/>
+      <c r="I5" s="109"/>
+      <c r="J5" s="110"/>
+    </row>
+    <row r="6" spans="1:10" ht="31.2">
+      <c r="A6" s="121"/>
       <c r="B6" s="62" t="s">
         <v>642</v>
       </c>
-      <c r="C6" s="112">
+      <c r="C6" s="111">
         <v>3</v>
       </c>
-      <c r="D6" s="107"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="109" t="s">
+      <c r="D6" s="106"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="108" t="s">
         <v>643</v>
       </c>
-      <c r="G6" s="110"/>
-      <c r="H6" s="110"/>
-      <c r="I6" s="110"/>
-      <c r="J6" s="111"/>
+      <c r="G6" s="109"/>
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="110"/>
     </row>
     <row r="7" spans="1:10" ht="48" customHeight="1">
-      <c r="A7" s="121" t="s">
+      <c r="A7" s="120" t="s">
         <v>644</v>
       </c>
       <c r="B7" s="62" t="s">
         <v>645</v>
       </c>
-      <c r="C7" s="113">
-        <v>1</v>
-      </c>
-      <c r="D7" s="107">
+      <c r="C7" s="112">
+        <v>1</v>
+      </c>
+      <c r="D7" s="106">
         <v>1026</v>
       </c>
-      <c r="E7" s="108"/>
-      <c r="F7" s="109" t="s">
+      <c r="E7" s="107"/>
+      <c r="F7" s="108" t="s">
         <v>646</v>
       </c>
-      <c r="G7" s="110"/>
-      <c r="H7" s="110"/>
-      <c r="I7" s="110"/>
-      <c r="J7" s="111"/>
-    </row>
-    <row r="8" spans="1:10" ht="31.5">
-      <c r="A8" s="121"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="109"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="110"/>
+    </row>
+    <row r="8" spans="1:10" ht="31.2">
+      <c r="A8" s="120"/>
       <c r="B8" s="62" t="s">
         <v>647</v>
       </c>
-      <c r="C8" s="113">
-        <v>1</v>
-      </c>
-      <c r="D8" s="107">
+      <c r="C8" s="112">
+        <v>1</v>
+      </c>
+      <c r="D8" s="106">
         <v>1002</v>
       </c>
-      <c r="E8" s="108"/>
-      <c r="F8" s="109" t="s">
+      <c r="E8" s="107"/>
+      <c r="F8" s="108" t="s">
         <v>648</v>
       </c>
-      <c r="G8" s="110"/>
-      <c r="H8" s="110"/>
-      <c r="I8" s="110"/>
-      <c r="J8" s="111"/>
-    </row>
-    <row r="9" spans="1:10" ht="47.25">
-      <c r="A9" s="121"/>
+      <c r="G8" s="109"/>
+      <c r="H8" s="109"/>
+      <c r="I8" s="109"/>
+      <c r="J8" s="110"/>
+    </row>
+    <row r="9" spans="1:10" ht="46.8">
+      <c r="A9" s="120"/>
       <c r="B9" s="62" t="s">
         <v>649</v>
       </c>
-      <c r="C9" s="113">
-        <v>1</v>
-      </c>
-      <c r="D9" s="107">
+      <c r="C9" s="112">
+        <v>1</v>
+      </c>
+      <c r="D9" s="106">
         <v>829</v>
       </c>
-      <c r="E9" s="108"/>
-      <c r="F9" s="109" t="s">
+      <c r="E9" s="107"/>
+      <c r="F9" s="108" t="s">
         <v>650</v>
       </c>
-      <c r="G9" s="110"/>
-      <c r="H9" s="110"/>
-      <c r="I9" s="110"/>
-      <c r="J9" s="111"/>
-    </row>
-    <row r="10" spans="1:10" ht="47.25">
-      <c r="A10" s="121"/>
+      <c r="G9" s="109"/>
+      <c r="H9" s="109"/>
+      <c r="I9" s="109"/>
+      <c r="J9" s="110"/>
+    </row>
+    <row r="10" spans="1:10" ht="46.8">
+      <c r="A10" s="120"/>
       <c r="B10" s="62" t="s">
         <v>651</v>
       </c>
-      <c r="C10" s="106">
-        <v>2</v>
-      </c>
-      <c r="D10" s="107">
+      <c r="C10" s="105">
+        <v>2</v>
+      </c>
+      <c r="D10" s="106">
         <v>829</v>
       </c>
-      <c r="E10" s="108"/>
-      <c r="F10" s="109" t="s">
+      <c r="E10" s="107"/>
+      <c r="F10" s="108" t="s">
         <v>652</v>
       </c>
-      <c r="G10" s="110"/>
-      <c r="H10" s="110"/>
-      <c r="I10" s="110"/>
-      <c r="J10" s="111"/>
-    </row>
-    <row r="11" spans="1:10" ht="31.5">
-      <c r="A11" s="121"/>
+      <c r="G10" s="109"/>
+      <c r="H10" s="109"/>
+      <c r="I10" s="109"/>
+      <c r="J10" s="110"/>
+    </row>
+    <row r="11" spans="1:10" ht="31.2">
+      <c r="A11" s="120"/>
       <c r="B11" s="62" t="s">
         <v>653</v>
       </c>
-      <c r="C11" s="106">
-        <v>2</v>
-      </c>
-      <c r="D11" s="107"/>
-      <c r="E11" s="108"/>
-      <c r="F11" s="109" t="s">
+      <c r="C11" s="105">
+        <v>2</v>
+      </c>
+      <c r="D11" s="106"/>
+      <c r="E11" s="107"/>
+      <c r="F11" s="108" t="s">
         <v>654</v>
       </c>
-      <c r="G11" s="110"/>
-      <c r="H11" s="110"/>
-      <c r="I11" s="110"/>
-      <c r="J11" s="111"/>
-    </row>
-    <row r="12" spans="1:10" ht="47.25">
-      <c r="A12" s="121"/>
+      <c r="G11" s="109"/>
+      <c r="H11" s="109"/>
+      <c r="I11" s="109"/>
+      <c r="J11" s="110"/>
+    </row>
+    <row r="12" spans="1:10" ht="46.8">
+      <c r="A12" s="120"/>
       <c r="B12" s="62" t="s">
         <v>655</v>
       </c>
-      <c r="C12" s="106">
-        <v>2</v>
-      </c>
-      <c r="D12" s="107">
+      <c r="C12" s="105">
+        <v>2</v>
+      </c>
+      <c r="D12" s="106">
         <v>265</v>
       </c>
-      <c r="E12" s="108"/>
-      <c r="F12" s="109" t="s">
+      <c r="E12" s="107"/>
+      <c r="F12" s="108" t="s">
         <v>656</v>
       </c>
-      <c r="G12" s="110"/>
-      <c r="H12" s="110"/>
-      <c r="I12" s="110"/>
-      <c r="J12" s="111"/>
+      <c r="G12" s="109"/>
+      <c r="H12" s="109"/>
+      <c r="I12" s="109"/>
+      <c r="J12" s="110"/>
     </row>
     <row r="13" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A13" s="121" t="s">
+      <c r="A13" s="120" t="s">
         <v>657</v>
       </c>
       <c r="B13" s="62" t="s">
         <v>658</v>
       </c>
-      <c r="C13" s="113">
-        <v>1</v>
-      </c>
-      <c r="D13" s="107">
+      <c r="C13" s="112">
+        <v>1</v>
+      </c>
+      <c r="D13" s="106">
         <v>209</v>
       </c>
-      <c r="E13" s="108"/>
-      <c r="F13" s="109" t="s">
+      <c r="E13" s="107"/>
+      <c r="F13" s="108" t="s">
         <v>659</v>
       </c>
-      <c r="G13" s="110" t="s">
+      <c r="G13" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="H13" s="110"/>
-      <c r="I13" s="110"/>
-      <c r="J13" s="111"/>
-    </row>
-    <row r="14" spans="1:10" ht="47.25">
-      <c r="A14" s="121"/>
+      <c r="H13" s="109"/>
+      <c r="I13" s="109"/>
+      <c r="J13" s="110"/>
+    </row>
+    <row r="14" spans="1:10" ht="46.8">
+      <c r="A14" s="120"/>
       <c r="B14" s="62" t="s">
         <v>660</v>
       </c>
-      <c r="C14" s="113">
-        <v>1</v>
-      </c>
-      <c r="D14" s="107">
+      <c r="C14" s="112">
+        <v>1</v>
+      </c>
+      <c r="D14" s="106">
         <v>497</v>
       </c>
-      <c r="E14" s="108"/>
-      <c r="F14" s="109" t="s">
+      <c r="E14" s="107"/>
+      <c r="F14" s="108" t="s">
         <v>661</v>
       </c>
-      <c r="G14" s="110"/>
-      <c r="H14" s="110"/>
-      <c r="I14" s="110"/>
-      <c r="J14" s="111"/>
-    </row>
-    <row r="15" spans="1:10" ht="31.5">
-      <c r="A15" s="121"/>
+      <c r="G14" s="109"/>
+      <c r="H14" s="109"/>
+      <c r="I14" s="109"/>
+      <c r="J14" s="110"/>
+    </row>
+    <row r="15" spans="1:10" ht="31.2">
+      <c r="A15" s="120"/>
       <c r="B15" s="62" t="s">
         <v>662</v>
       </c>
-      <c r="C15" s="113">
-        <v>1</v>
-      </c>
-      <c r="D15" s="107">
+      <c r="C15" s="112">
+        <v>1</v>
+      </c>
+      <c r="D15" s="106">
         <v>200</v>
       </c>
-      <c r="E15" s="108"/>
-      <c r="F15" s="109" t="s">
+      <c r="E15" s="107"/>
+      <c r="F15" s="108" t="s">
         <v>663</v>
       </c>
-      <c r="G15" s="110"/>
-      <c r="H15" s="110"/>
-      <c r="I15" s="110"/>
-      <c r="J15" s="111"/>
+      <c r="G15" s="109"/>
+      <c r="H15" s="109"/>
+      <c r="I15" s="109"/>
+      <c r="J15" s="110"/>
     </row>
     <row r="16" spans="1:10" ht="48" customHeight="1">
-      <c r="A16" s="121" t="s">
+      <c r="A16" s="120" t="s">
         <v>664</v>
       </c>
       <c r="B16" s="62" t="s">
         <v>665</v>
       </c>
-      <c r="C16" s="113">
-        <v>1</v>
-      </c>
-      <c r="D16" s="107">
+      <c r="C16" s="112">
+        <v>1</v>
+      </c>
+      <c r="D16" s="106">
         <v>173</v>
       </c>
-      <c r="E16" s="108"/>
-      <c r="F16" s="109" t="s">
+      <c r="E16" s="107"/>
+      <c r="F16" s="108" t="s">
         <v>666</v>
       </c>
-      <c r="G16" s="110"/>
-      <c r="H16" s="110"/>
-      <c r="I16" s="110"/>
-      <c r="J16" s="111"/>
-    </row>
-    <row r="17" spans="1:10" ht="31.5">
-      <c r="A17" s="121"/>
+      <c r="G16" s="109"/>
+      <c r="H16" s="109"/>
+      <c r="I16" s="109"/>
+      <c r="J16" s="110"/>
+    </row>
+    <row r="17" spans="1:10" ht="31.2">
+      <c r="A17" s="120"/>
       <c r="B17" s="62" t="s">
         <v>667</v>
       </c>
-      <c r="C17" s="113">
-        <v>1</v>
-      </c>
-      <c r="D17" s="107">
+      <c r="C17" s="112">
+        <v>1</v>
+      </c>
+      <c r="D17" s="106">
         <v>116</v>
       </c>
-      <c r="E17" s="108"/>
-      <c r="F17" s="109" t="s">
+      <c r="E17" s="107"/>
+      <c r="F17" s="108" t="s">
         <v>668</v>
       </c>
-      <c r="G17" s="110"/>
-      <c r="H17" s="110"/>
-      <c r="I17" s="110"/>
-      <c r="J17" s="111"/>
-    </row>
-    <row r="18" spans="1:10" ht="31.5">
-      <c r="A18" s="121"/>
+      <c r="G17" s="109"/>
+      <c r="H17" s="109"/>
+      <c r="I17" s="109"/>
+      <c r="J17" s="110"/>
+    </row>
+    <row r="18" spans="1:10" ht="31.2">
+      <c r="A18" s="120"/>
       <c r="B18" s="62" t="s">
         <v>669</v>
       </c>
-      <c r="C18" s="113">
-        <v>1</v>
-      </c>
-      <c r="D18" s="107">
+      <c r="C18" s="112">
+        <v>1</v>
+      </c>
+      <c r="D18" s="106">
         <v>1021</v>
       </c>
-      <c r="E18" s="108"/>
-      <c r="F18" s="109" t="s">
+      <c r="E18" s="107"/>
+      <c r="F18" s="108" t="s">
         <v>670</v>
       </c>
-      <c r="G18" s="110"/>
-      <c r="H18" s="110"/>
-      <c r="I18" s="110"/>
-      <c r="J18" s="111"/>
-    </row>
-    <row r="19" spans="1:10" ht="15.75">
-      <c r="A19" s="121"/>
+      <c r="G18" s="109"/>
+      <c r="H18" s="109"/>
+      <c r="I18" s="109"/>
+      <c r="J18" s="110"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.6">
+      <c r="A19" s="120"/>
       <c r="B19" s="62" t="s">
         <v>671</v>
       </c>
-      <c r="C19" s="113">
-        <v>1</v>
-      </c>
-      <c r="D19" s="107">
+      <c r="C19" s="112">
+        <v>1</v>
+      </c>
+      <c r="D19" s="106">
         <v>116</v>
       </c>
-      <c r="E19" s="108"/>
-      <c r="F19" s="109" t="s">
+      <c r="E19" s="107"/>
+      <c r="F19" s="108" t="s">
         <v>672</v>
       </c>
-      <c r="G19" s="110"/>
-      <c r="H19" s="110"/>
-      <c r="I19" s="110"/>
-      <c r="J19" s="111"/>
-    </row>
-    <row r="20" spans="1:10" ht="31.5">
-      <c r="A20" s="121"/>
+      <c r="G19" s="109"/>
+      <c r="H19" s="109"/>
+      <c r="I19" s="109"/>
+      <c r="J19" s="110"/>
+    </row>
+    <row r="20" spans="1:10" ht="31.2">
+      <c r="A20" s="120"/>
       <c r="B20" s="62" t="s">
         <v>673</v>
       </c>
-      <c r="C20" s="113">
-        <v>1</v>
-      </c>
-      <c r="D20" s="107">
+      <c r="C20" s="112">
+        <v>1</v>
+      </c>
+      <c r="D20" s="106">
         <v>523</v>
       </c>
-      <c r="E20" s="108"/>
-      <c r="F20" s="109" t="s">
+      <c r="E20" s="107"/>
+      <c r="F20" s="108" t="s">
         <v>674</v>
       </c>
-      <c r="G20" s="110"/>
-      <c r="H20" s="110"/>
-      <c r="I20" s="110"/>
-      <c r="J20" s="111"/>
-    </row>
-    <row r="21" spans="1:10" ht="31.5">
-      <c r="A21" s="121"/>
+      <c r="G20" s="109"/>
+      <c r="H20" s="109"/>
+      <c r="I20" s="109"/>
+      <c r="J20" s="110"/>
+    </row>
+    <row r="21" spans="1:10" ht="31.2">
+      <c r="A21" s="120"/>
       <c r="B21" s="62" t="s">
         <v>675</v>
       </c>
-      <c r="C21" s="113">
-        <v>1</v>
-      </c>
-      <c r="D21" s="107">
+      <c r="C21" s="112">
+        <v>1</v>
+      </c>
+      <c r="D21" s="106">
         <v>116</v>
       </c>
-      <c r="E21" s="108"/>
-      <c r="F21" s="109" t="s">
+      <c r="E21" s="107"/>
+      <c r="F21" s="108" t="s">
         <v>676</v>
       </c>
-      <c r="G21" s="110"/>
-      <c r="H21" s="110"/>
-      <c r="I21" s="110"/>
-      <c r="J21" s="111"/>
-    </row>
-    <row r="22" spans="1:10" ht="63">
-      <c r="A22" s="121"/>
+      <c r="G21" s="109"/>
+      <c r="H21" s="109"/>
+      <c r="I21" s="109"/>
+      <c r="J21" s="110"/>
+    </row>
+    <row r="22" spans="1:10" ht="62.4">
+      <c r="A22" s="120"/>
       <c r="B22" s="62" t="s">
         <v>677</v>
       </c>
-      <c r="C22" s="113">
-        <v>1</v>
-      </c>
-      <c r="D22" s="107">
+      <c r="C22" s="112">
+        <v>1</v>
+      </c>
+      <c r="D22" s="106">
         <v>1021</v>
       </c>
-      <c r="E22" s="108"/>
-      <c r="F22" s="109" t="s">
+      <c r="E22" s="107"/>
+      <c r="F22" s="108" t="s">
         <v>678</v>
       </c>
-      <c r="G22" s="110"/>
-      <c r="H22" s="110"/>
-      <c r="I22" s="110"/>
-      <c r="J22" s="111"/>
+      <c r="G22" s="109"/>
+      <c r="H22" s="109"/>
+      <c r="I22" s="109"/>
+      <c r="J22" s="110"/>
     </row>
     <row r="23" spans="1:10" ht="48" customHeight="1">
-      <c r="A23" s="121" t="s">
+      <c r="A23" s="120" t="s">
         <v>679</v>
       </c>
       <c r="B23" s="62" t="s">
         <v>680</v>
       </c>
-      <c r="C23" s="113">
-        <v>1</v>
-      </c>
-      <c r="D23" s="107">
+      <c r="C23" s="112">
+        <v>1</v>
+      </c>
+      <c r="D23" s="106">
         <v>749</v>
       </c>
-      <c r="E23" s="108"/>
-      <c r="F23" s="109" t="s">
+      <c r="E23" s="107"/>
+      <c r="F23" s="108" t="s">
         <v>681</v>
       </c>
-      <c r="G23" s="110"/>
-      <c r="H23" s="110"/>
-      <c r="I23" s="110"/>
-      <c r="J23" s="111"/>
-    </row>
-    <row r="24" spans="1:10" ht="31.5">
-      <c r="A24" s="121"/>
+      <c r="G23" s="109"/>
+      <c r="H23" s="109"/>
+      <c r="I23" s="109"/>
+      <c r="J23" s="110"/>
+    </row>
+    <row r="24" spans="1:10" ht="31.2">
+      <c r="A24" s="120"/>
       <c r="B24" s="62" t="s">
         <v>682</v>
       </c>
-      <c r="C24" s="113">
-        <v>1</v>
-      </c>
-      <c r="D24" s="107">
+      <c r="C24" s="112">
+        <v>1</v>
+      </c>
+      <c r="D24" s="106">
         <v>346</v>
       </c>
-      <c r="E24" s="108"/>
-      <c r="F24" s="109" t="s">
+      <c r="E24" s="107"/>
+      <c r="F24" s="108" t="s">
         <v>683</v>
       </c>
-      <c r="G24" s="110"/>
-      <c r="H24" s="110"/>
-      <c r="I24" s="110"/>
-      <c r="J24" s="111"/>
-    </row>
-    <row r="25" spans="1:10" ht="47.25">
-      <c r="A25" s="121"/>
+      <c r="G24" s="109"/>
+      <c r="H24" s="109"/>
+      <c r="I24" s="109"/>
+      <c r="J24" s="110"/>
+    </row>
+    <row r="25" spans="1:10" ht="46.8">
+      <c r="A25" s="120"/>
       <c r="B25" s="62" t="s">
         <v>684</v>
       </c>
-      <c r="C25" s="113">
-        <v>1</v>
-      </c>
-      <c r="D25" s="107">
+      <c r="C25" s="112">
+        <v>1</v>
+      </c>
+      <c r="D25" s="106">
         <v>346</v>
       </c>
-      <c r="E25" s="108"/>
-      <c r="F25" s="109" t="s">
+      <c r="E25" s="107"/>
+      <c r="F25" s="108" t="s">
         <v>685</v>
       </c>
-      <c r="G25" s="110"/>
-      <c r="H25" s="110"/>
-      <c r="I25" s="110"/>
-      <c r="J25" s="111"/>
-    </row>
-    <row r="26" spans="1:10" ht="31.5">
-      <c r="A26" s="121"/>
+      <c r="G25" s="109"/>
+      <c r="H25" s="109"/>
+      <c r="I25" s="109"/>
+      <c r="J25" s="110"/>
+    </row>
+    <row r="26" spans="1:10" ht="31.2">
+      <c r="A26" s="120"/>
       <c r="B26" s="62" t="s">
         <v>686</v>
       </c>
-      <c r="C26" s="114">
-        <v>2</v>
-      </c>
-      <c r="D26" s="115">
+      <c r="C26" s="113">
+        <v>2</v>
+      </c>
+      <c r="D26" s="114">
         <v>306</v>
       </c>
-      <c r="E26" s="116"/>
-      <c r="F26" s="117" t="s">
+      <c r="E26" s="115"/>
+      <c r="F26" s="116" t="s">
         <v>687</v>
       </c>
-      <c r="G26" s="118"/>
-      <c r="H26" s="118"/>
-      <c r="I26" s="118"/>
-      <c r="J26" s="119"/>
+      <c r="G26" s="117"/>
+      <c r="H26" s="117"/>
+      <c r="I26" s="117"/>
+      <c r="J26" s="118"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -6497,22 +6568,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="15"/>
-    <col min="3" max="3" width="10.7109375" style="15" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="15"/>
-    <col min="6" max="6" width="60.85546875" style="15" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" style="15" customWidth="1"/>
+    <col min="1" max="1" width="35.44140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="15"/>
+    <col min="3" max="3" width="10.6640625" style="15" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="15"/>
+    <col min="6" max="6" width="60.88671875" style="15" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" style="15" customWidth="1"/>
     <col min="8" max="8" width="36" style="15" customWidth="1"/>
-    <col min="9" max="9" width="31.7109375" style="15" customWidth="1"/>
-    <col min="10" max="10" width="41.7109375" style="15" customWidth="1"/>
-    <col min="11" max="1024" width="8.85546875" style="15"/>
+    <col min="9" max="9" width="31.6640625" style="15" customWidth="1"/>
+    <col min="10" max="10" width="41.6640625" style="15" customWidth="1"/>
+    <col min="11" max="1024" width="8.88671875" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" ht="42">
@@ -6547,8 +6618,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="25" customFormat="1" ht="58.15" customHeight="1">
-      <c r="A2" s="120" t="s">
+    <row r="2" spans="1:10" s="25" customFormat="1" ht="58.2" customHeight="1">
+      <c r="A2" s="119" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -6573,8 +6644,8 @@
       </c>
       <c r="J2" s="24"/>
     </row>
-    <row r="3" spans="1:10" s="25" customFormat="1" ht="63">
-      <c r="A3" s="120"/>
+    <row r="3" spans="1:10" s="25" customFormat="1" ht="62.4">
+      <c r="A3" s="119"/>
       <c r="B3" s="19" t="s">
         <v>33</v>
       </c>
@@ -6601,8 +6672,8 @@
         <v>690</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="25" customFormat="1" ht="63">
-      <c r="A4" s="120"/>
+    <row r="4" spans="1:10" s="25" customFormat="1" ht="62.4">
+      <c r="A4" s="119"/>
       <c r="B4" s="19" t="s">
         <v>35</v>
       </c>
@@ -6627,8 +6698,8 @@
       </c>
       <c r="J4" s="31"/>
     </row>
-    <row r="5" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A5" s="120"/>
+    <row r="5" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A5" s="119"/>
       <c r="B5" s="19" t="s">
         <v>37</v>
       </c>
@@ -6655,8 +6726,8 @@
         <v>690</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="25" customFormat="1" ht="63">
-      <c r="A6" s="120"/>
+    <row r="6" spans="1:10" s="25" customFormat="1" ht="62.4">
+      <c r="A6" s="119"/>
       <c r="B6" s="19" t="s">
         <v>39</v>
       </c>
@@ -6683,8 +6754,8 @@
         <v>690</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="25" customFormat="1" ht="78.75">
-      <c r="A7" s="120"/>
+    <row r="7" spans="1:10" s="25" customFormat="1" ht="78">
+      <c r="A7" s="119"/>
       <c r="B7" s="19" t="s">
         <v>41</v>
       </c>
@@ -6703,8 +6774,8 @@
       <c r="I7" s="30"/>
       <c r="J7" s="31"/>
     </row>
-    <row r="8" spans="1:10" s="25" customFormat="1" ht="47.25">
-      <c r="A8" s="120"/>
+    <row r="8" spans="1:10" s="25" customFormat="1" ht="46.8">
+      <c r="A8" s="119"/>
       <c r="B8" s="19" t="s">
         <v>43</v>
       </c>
@@ -6730,7 +6801,7 @@
       <c r="J8" s="31"/>
     </row>
     <row r="9" spans="1:10" s="25" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A9" s="120" t="s">
+      <c r="A9" s="119" t="s">
         <v>45</v>
       </c>
       <c r="B9" s="19" t="s">
@@ -6757,8 +6828,8 @@
       </c>
       <c r="J9" s="31"/>
     </row>
-    <row r="10" spans="1:10" s="25" customFormat="1" ht="78.75">
-      <c r="A10" s="120"/>
+    <row r="10" spans="1:10" s="25" customFormat="1" ht="78">
+      <c r="A10" s="119"/>
       <c r="B10" s="19" t="s">
         <v>48</v>
       </c>
@@ -6783,8 +6854,8 @@
       </c>
       <c r="J10" s="31"/>
     </row>
-    <row r="11" spans="1:10" s="25" customFormat="1" ht="63">
-      <c r="A11" s="120"/>
+    <row r="11" spans="1:10" s="25" customFormat="1" ht="62.4">
+      <c r="A11" s="119"/>
       <c r="B11" s="19" t="s">
         <v>50</v>
       </c>
@@ -6809,8 +6880,8 @@
       </c>
       <c r="J11" s="31"/>
     </row>
-    <row r="12" spans="1:10" s="25" customFormat="1" ht="63">
-      <c r="A12" s="120"/>
+    <row r="12" spans="1:10" s="25" customFormat="1" ht="62.4">
+      <c r="A12" s="119"/>
       <c r="B12" s="19" t="s">
         <v>52</v>
       </c>
@@ -6850,7 +6921,7 @@
       <c r="J13" s="31"/>
     </row>
     <row r="14" spans="1:10" s="25" customFormat="1" ht="48" customHeight="1">
-      <c r="A14" s="120" t="s">
+      <c r="A14" s="119" t="s">
         <v>57</v>
       </c>
       <c r="B14" s="19" t="s">
@@ -6871,8 +6942,8 @@
       <c r="I14" s="28"/>
       <c r="J14" s="32"/>
     </row>
-    <row r="15" spans="1:10" s="25" customFormat="1" ht="15.75">
-      <c r="A15" s="120"/>
+    <row r="15" spans="1:10" s="25" customFormat="1" ht="15.6">
+      <c r="A15" s="119"/>
       <c r="B15" s="19" t="s">
         <v>60</v>
       </c>
@@ -6893,8 +6964,8 @@
       <c r="I15" s="28"/>
       <c r="J15" s="32"/>
     </row>
-    <row r="16" spans="1:10" s="25" customFormat="1" ht="15.75">
-      <c r="A16" s="120"/>
+    <row r="16" spans="1:10" s="25" customFormat="1" ht="15.6">
+      <c r="A16" s="119"/>
       <c r="B16" s="19" t="s">
         <v>62</v>
       </c>
@@ -6915,8 +6986,8 @@
       <c r="I16" s="28"/>
       <c r="J16" s="32"/>
     </row>
-    <row r="17" spans="1:10" s="25" customFormat="1" ht="94.5">
-      <c r="A17" s="120"/>
+    <row r="17" spans="1:10" s="25" customFormat="1" ht="93.6">
+      <c r="A17" s="119"/>
       <c r="B17" s="19" t="s">
         <v>64</v>
       </c>
@@ -6935,8 +7006,8 @@
       <c r="I17" s="28"/>
       <c r="J17" s="32"/>
     </row>
-    <row r="18" spans="1:10" s="25" customFormat="1" ht="94.5">
-      <c r="A18" s="120"/>
+    <row r="18" spans="1:10" s="25" customFormat="1" ht="93.6">
+      <c r="A18" s="119"/>
       <c r="B18" s="19" t="s">
         <v>66</v>
       </c>
@@ -6962,7 +7033,7 @@
       <c r="J18" s="32"/>
     </row>
     <row r="19" spans="1:10" s="25" customFormat="1" ht="48" customHeight="1">
-      <c r="A19" s="120" t="s">
+      <c r="A19" s="119" t="s">
         <v>68</v>
       </c>
       <c r="B19" s="19" t="s">
@@ -6989,8 +7060,8 @@
       </c>
       <c r="J19" s="32"/>
     </row>
-    <row r="20" spans="1:10" s="25" customFormat="1" ht="78.75">
-      <c r="A20" s="120"/>
+    <row r="20" spans="1:10" s="25" customFormat="1" ht="78">
+      <c r="A20" s="119"/>
       <c r="B20" s="19" t="s">
         <v>71</v>
       </c>
@@ -7015,8 +7086,8 @@
       </c>
       <c r="J20" s="32"/>
     </row>
-    <row r="21" spans="1:10" s="25" customFormat="1" ht="47.25">
-      <c r="A21" s="120"/>
+    <row r="21" spans="1:10" s="25" customFormat="1" ht="46.8">
+      <c r="A21" s="119"/>
       <c r="B21" s="19" t="s">
         <v>73</v>
       </c>
@@ -7035,8 +7106,8 @@
       <c r="I21" s="28"/>
       <c r="J21" s="32"/>
     </row>
-    <row r="22" spans="1:10" s="25" customFormat="1" ht="63">
-      <c r="A22" s="120"/>
+    <row r="22" spans="1:10" s="25" customFormat="1" ht="62.4">
+      <c r="A22" s="119"/>
       <c r="B22" s="19" t="s">
         <v>75</v>
       </c>
@@ -7056,7 +7127,7 @@
       <c r="J22" s="32"/>
     </row>
     <row r="23" spans="1:10" s="25" customFormat="1" ht="48" customHeight="1">
-      <c r="A23" s="120" t="s">
+      <c r="A23" s="119" t="s">
         <v>77</v>
       </c>
       <c r="B23" s="19" t="s">
@@ -7079,8 +7150,8 @@
       <c r="I23" s="28"/>
       <c r="J23" s="32"/>
     </row>
-    <row r="24" spans="1:10" s="25" customFormat="1" ht="47.25">
-      <c r="A24" s="120"/>
+    <row r="24" spans="1:10" s="25" customFormat="1" ht="46.8">
+      <c r="A24" s="119"/>
       <c r="B24" s="19" t="s">
         <v>80</v>
       </c>
@@ -7101,8 +7172,8 @@
       <c r="I24" s="28"/>
       <c r="J24" s="32"/>
     </row>
-    <row r="25" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A25" s="120"/>
+    <row r="25" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A25" s="119"/>
       <c r="B25" s="19" t="s">
         <v>82</v>
       </c>
@@ -7121,8 +7192,8 @@
       <c r="I25" s="28"/>
       <c r="J25" s="32"/>
     </row>
-    <row r="26" spans="1:10" s="25" customFormat="1" ht="47.25">
-      <c r="A26" s="120"/>
+    <row r="26" spans="1:10" s="25" customFormat="1" ht="46.8">
+      <c r="A26" s="119"/>
       <c r="B26" s="19" t="s">
         <v>84</v>
       </c>
@@ -7148,7 +7219,7 @@
       <c r="J26" s="32"/>
     </row>
     <row r="27" spans="1:10" s="25" customFormat="1" ht="48" customHeight="1">
-      <c r="A27" s="120" t="s">
+      <c r="A27" s="119" t="s">
         <v>86</v>
       </c>
       <c r="B27" s="19" t="s">
@@ -7169,8 +7240,8 @@
       <c r="I27" s="28"/>
       <c r="J27" s="32"/>
     </row>
-    <row r="28" spans="1:10" s="25" customFormat="1" ht="63">
-      <c r="A28" s="120"/>
+    <row r="28" spans="1:10" s="25" customFormat="1" ht="62.4">
+      <c r="A28" s="119"/>
       <c r="B28" s="19" t="s">
         <v>89</v>
       </c>
@@ -7188,7 +7259,7 @@
       <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" s="25" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A29" s="120" t="s">
+      <c r="A29" s="119" t="s">
         <v>91</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -7207,8 +7278,8 @@
       <c r="I29" s="28"/>
       <c r="J29" s="32"/>
     </row>
-    <row r="30" spans="1:10" s="25" customFormat="1" ht="78.75">
-      <c r="A30" s="120"/>
+    <row r="30" spans="1:10" s="25" customFormat="1" ht="78">
+      <c r="A30" s="119"/>
       <c r="B30" s="19" t="s">
         <v>94</v>
       </c>
@@ -7226,7 +7297,7 @@
       <c r="J30" s="32"/>
     </row>
     <row r="31" spans="1:10" s="25" customFormat="1" ht="79.5" customHeight="1">
-      <c r="A31" s="120" t="s">
+      <c r="A31" s="119" t="s">
         <v>96</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -7247,8 +7318,8 @@
       <c r="I31" s="28"/>
       <c r="J31" s="32"/>
     </row>
-    <row r="32" spans="1:10" s="25" customFormat="1" ht="63">
-      <c r="A32" s="120"/>
+    <row r="32" spans="1:10" s="25" customFormat="1" ht="62.4">
+      <c r="A32" s="119"/>
       <c r="B32" s="19" t="s">
         <v>99</v>
       </c>
@@ -7267,7 +7338,7 @@
       <c r="I32" s="28"/>
       <c r="J32" s="32"/>
     </row>
-    <row r="33" spans="1:10" s="25" customFormat="1" ht="78.75">
+    <row r="33" spans="1:10" s="25" customFormat="1" ht="78">
       <c r="A33" s="2" t="s">
         <v>101</v>
       </c>
@@ -7290,7 +7361,7 @@
       <c r="J33" s="32"/>
     </row>
     <row r="34" spans="1:10" s="25" customFormat="1" ht="48" customHeight="1">
-      <c r="A34" s="120" t="s">
+      <c r="A34" s="119" t="s">
         <v>104</v>
       </c>
       <c r="B34" s="19" t="s">
@@ -7317,8 +7388,8 @@
       </c>
       <c r="J34" s="32"/>
     </row>
-    <row r="35" spans="1:10" s="25" customFormat="1" ht="47.25">
-      <c r="A35" s="120"/>
+    <row r="35" spans="1:10" s="25" customFormat="1" ht="46.8">
+      <c r="A35" s="119"/>
       <c r="B35" s="19" t="s">
         <v>107</v>
       </c>
@@ -7337,8 +7408,8 @@
       <c r="I35" s="28"/>
       <c r="J35" s="32"/>
     </row>
-    <row r="36" spans="1:10" s="25" customFormat="1" ht="63">
-      <c r="A36" s="120"/>
+    <row r="36" spans="1:10" s="25" customFormat="1" ht="62.4">
+      <c r="A36" s="119"/>
       <c r="B36" s="19" t="s">
         <v>109</v>
       </c>
@@ -7358,7 +7429,7 @@
       <c r="J36" s="32"/>
     </row>
     <row r="37" spans="1:10" s="25" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A37" s="120" t="s">
+      <c r="A37" s="119" t="s">
         <v>111</v>
       </c>
       <c r="B37" s="19" t="s">
@@ -7381,8 +7452,8 @@
       <c r="I37" s="28"/>
       <c r="J37" s="32"/>
     </row>
-    <row r="38" spans="1:10" s="25" customFormat="1" ht="94.5">
-      <c r="A38" s="120"/>
+    <row r="38" spans="1:10" s="25" customFormat="1" ht="93.6">
+      <c r="A38" s="119"/>
       <c r="B38" s="19" t="s">
         <v>114</v>
       </c>
@@ -7419,8 +7490,8 @@
       <c r="I39" s="28"/>
       <c r="J39" s="32"/>
     </row>
-    <row r="40" spans="1:10" s="25" customFormat="1" ht="58.9" customHeight="1">
-      <c r="A40" s="120" t="s">
+    <row r="40" spans="1:10" s="25" customFormat="1" ht="58.95" customHeight="1">
+      <c r="A40" s="119" t="s">
         <v>117</v>
       </c>
       <c r="B40" s="19" t="s">
@@ -7441,8 +7512,8 @@
       <c r="I40" s="28"/>
       <c r="J40" s="32"/>
     </row>
-    <row r="41" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A41" s="120"/>
+    <row r="41" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A41" s="119"/>
       <c r="B41" s="19" t="s">
         <v>120</v>
       </c>
@@ -7461,8 +7532,8 @@
       <c r="I41" s="28"/>
       <c r="J41" s="32"/>
     </row>
-    <row r="42" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A42" s="120"/>
+    <row r="42" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A42" s="119"/>
       <c r="B42" s="19" t="s">
         <v>122</v>
       </c>
@@ -7481,8 +7552,8 @@
       <c r="I42" s="28"/>
       <c r="J42" s="32"/>
     </row>
-    <row r="43" spans="1:10" s="25" customFormat="1" ht="63">
-      <c r="A43" s="120"/>
+    <row r="43" spans="1:10" s="25" customFormat="1" ht="62.4">
+      <c r="A43" s="119"/>
       <c r="B43" s="19" t="s">
         <v>124</v>
       </c>
@@ -7499,8 +7570,8 @@
       <c r="I43" s="28"/>
       <c r="J43" s="32"/>
     </row>
-    <row r="44" spans="1:10" s="25" customFormat="1" ht="94.5">
-      <c r="A44" s="120"/>
+    <row r="44" spans="1:10" s="25" customFormat="1" ht="93.6">
+      <c r="A44" s="119"/>
       <c r="B44" s="19" t="s">
         <v>126</v>
       </c>
@@ -7519,8 +7590,8 @@
       <c r="I44" s="28"/>
       <c r="J44" s="32"/>
     </row>
-    <row r="45" spans="1:10" s="25" customFormat="1" ht="63">
-      <c r="A45" s="120"/>
+    <row r="45" spans="1:10" s="25" customFormat="1" ht="62.4">
+      <c r="A45" s="119"/>
       <c r="B45" s="19" t="s">
         <v>128</v>
       </c>
@@ -7541,17 +7612,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A26"/>
     <mergeCell ref="A40:A45"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A26"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="G2:G45" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -7572,22 +7643,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ58"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="38"/>
-    <col min="3" max="3" width="14.85546875" style="39" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="39"/>
+    <col min="1" max="1" width="34.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="38"/>
+    <col min="3" max="3" width="14.88671875" style="39" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="39"/>
     <col min="6" max="6" width="73" style="15" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" style="15" customWidth="1"/>
-    <col min="8" max="8" width="30.28515625" style="15" customWidth="1"/>
-    <col min="9" max="9" width="33.42578125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="25.44140625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="30.33203125" style="15" customWidth="1"/>
+    <col min="9" max="9" width="33.44140625" style="15" customWidth="1"/>
     <col min="10" max="10" width="29" style="15" customWidth="1"/>
-    <col min="11" max="1024" width="8.85546875" style="15"/>
+    <col min="11" max="1024" width="8.88671875" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="43" customFormat="1">
@@ -7623,7 +7694,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="25" customFormat="1" ht="48" customHeight="1">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="120" t="s">
         <v>130</v>
       </c>
       <c r="B2" s="44" t="s">
@@ -7646,8 +7717,8 @@
       <c r="I2" s="50"/>
       <c r="J2" s="51"/>
     </row>
-    <row r="3" spans="1:10" s="25" customFormat="1" ht="47.25">
-      <c r="A3" s="121"/>
+    <row r="3" spans="1:10" s="25" customFormat="1" ht="46.8">
+      <c r="A3" s="120"/>
       <c r="B3" s="44" t="s">
         <v>134</v>
       </c>
@@ -7668,8 +7739,8 @@
       <c r="I3" s="30"/>
       <c r="J3" s="31"/>
     </row>
-    <row r="4" spans="1:10" s="25" customFormat="1" ht="47.25">
-      <c r="A4" s="121"/>
+    <row r="4" spans="1:10" s="25" customFormat="1" ht="46.8">
+      <c r="A4" s="120"/>
       <c r="B4" s="44" t="s">
         <v>136</v>
       </c>
@@ -7690,8 +7761,8 @@
       <c r="I4" s="30"/>
       <c r="J4" s="31"/>
     </row>
-    <row r="5" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A5" s="121"/>
+    <row r="5" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A5" s="120"/>
       <c r="B5" s="44" t="s">
         <v>138</v>
       </c>
@@ -7712,8 +7783,8 @@
       <c r="I5" s="30"/>
       <c r="J5" s="31"/>
     </row>
-    <row r="6" spans="1:10" s="25" customFormat="1" ht="15.75">
-      <c r="A6" s="121"/>
+    <row r="6" spans="1:10" s="25" customFormat="1" ht="15.6">
+      <c r="A6" s="120"/>
       <c r="B6" s="44" t="s">
         <v>140</v>
       </c>
@@ -7734,8 +7805,8 @@
       <c r="I6" s="30"/>
       <c r="J6" s="31"/>
     </row>
-    <row r="7" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A7" s="121"/>
+    <row r="7" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A7" s="120"/>
       <c r="B7" s="44" t="s">
         <v>142</v>
       </c>
@@ -7756,8 +7827,8 @@
       <c r="I7" s="30"/>
       <c r="J7" s="31"/>
     </row>
-    <row r="8" spans="1:10" s="25" customFormat="1" ht="141.75">
-      <c r="A8" s="121"/>
+    <row r="8" spans="1:10" s="25" customFormat="1" ht="140.4">
+      <c r="A8" s="120"/>
       <c r="B8" s="44" t="s">
         <v>144</v>
       </c>
@@ -7778,8 +7849,8 @@
       <c r="I8" s="30"/>
       <c r="J8" s="31"/>
     </row>
-    <row r="9" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A9" s="121"/>
+    <row r="9" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A9" s="120"/>
       <c r="B9" s="44" t="s">
         <v>146</v>
       </c>
@@ -7800,8 +7871,8 @@
       <c r="I9" s="30"/>
       <c r="J9" s="31"/>
     </row>
-    <row r="10" spans="1:10" s="25" customFormat="1" ht="63">
-      <c r="A10" s="121"/>
+    <row r="10" spans="1:10" s="25" customFormat="1" ht="62.4">
+      <c r="A10" s="120"/>
       <c r="B10" s="44" t="s">
         <v>148</v>
       </c>
@@ -7822,8 +7893,8 @@
       <c r="I10" s="30"/>
       <c r="J10" s="31"/>
     </row>
-    <row r="11" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A11" s="121"/>
+    <row r="11" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A11" s="120"/>
       <c r="B11" s="44" t="s">
         <v>150</v>
       </c>
@@ -7844,8 +7915,8 @@
       <c r="I11" s="30"/>
       <c r="J11" s="31"/>
     </row>
-    <row r="12" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A12" s="121"/>
+    <row r="12" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A12" s="120"/>
       <c r="B12" s="44" t="s">
         <v>152</v>
       </c>
@@ -7866,8 +7937,8 @@
       <c r="I12" s="30"/>
       <c r="J12" s="31"/>
     </row>
-    <row r="13" spans="1:10" s="25" customFormat="1" ht="47.25">
-      <c r="A13" s="121"/>
+    <row r="13" spans="1:10" s="25" customFormat="1" ht="46.8">
+      <c r="A13" s="120"/>
       <c r="B13" s="44" t="s">
         <v>154</v>
       </c>
@@ -7889,7 +7960,7 @@
       <c r="J13" s="31"/>
     </row>
     <row r="14" spans="1:10" s="25" customFormat="1" ht="111" customHeight="1">
-      <c r="A14" s="121" t="s">
+      <c r="A14" s="120" t="s">
         <v>156</v>
       </c>
       <c r="B14" s="44" t="s">
@@ -7912,8 +7983,8 @@
       <c r="I14" s="30"/>
       <c r="J14" s="31"/>
     </row>
-    <row r="15" spans="1:10" s="25" customFormat="1" ht="78.75">
-      <c r="A15" s="121"/>
+    <row r="15" spans="1:10" s="25" customFormat="1" ht="93.6">
+      <c r="A15" s="120"/>
       <c r="B15" s="44" t="s">
         <v>160</v>
       </c>
@@ -7934,8 +8005,8 @@
       <c r="I15" s="30"/>
       <c r="J15" s="31"/>
     </row>
-    <row r="16" spans="1:10" s="25" customFormat="1" ht="94.5">
-      <c r="A16" s="121"/>
+    <row r="16" spans="1:10" s="25" customFormat="1" ht="93.6">
+      <c r="A16" s="120"/>
       <c r="B16" s="44" t="s">
         <v>163</v>
       </c>
@@ -7954,8 +8025,8 @@
       <c r="I16" s="30"/>
       <c r="J16" s="31"/>
     </row>
-    <row r="17" spans="1:10" s="25" customFormat="1" ht="63">
-      <c r="A17" s="121"/>
+    <row r="17" spans="1:10" s="25" customFormat="1" ht="62.4">
+      <c r="A17" s="120"/>
       <c r="B17" s="44" t="s">
         <v>165</v>
       </c>
@@ -7976,8 +8047,8 @@
       <c r="I17" s="30"/>
       <c r="J17" s="31"/>
     </row>
-    <row r="18" spans="1:10" s="25" customFormat="1" ht="47.25">
-      <c r="A18" s="121"/>
+    <row r="18" spans="1:10" s="25" customFormat="1" ht="46.8">
+      <c r="A18" s="120"/>
       <c r="B18" s="44" t="s">
         <v>168</v>
       </c>
@@ -7998,8 +8069,8 @@
       <c r="I18" s="30"/>
       <c r="J18" s="31"/>
     </row>
-    <row r="19" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A19" s="121"/>
+    <row r="19" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A19" s="120"/>
       <c r="B19" s="44" t="s">
         <v>171</v>
       </c>
@@ -8020,8 +8091,8 @@
       <c r="I19" s="30"/>
       <c r="J19" s="31"/>
     </row>
-    <row r="20" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A20" s="121"/>
+    <row r="20" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A20" s="120"/>
       <c r="B20" s="44" t="s">
         <v>174</v>
       </c>
@@ -8043,7 +8114,7 @@
       <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10" s="25" customFormat="1" ht="79.5" customHeight="1">
-      <c r="A21" s="121" t="s">
+      <c r="A21" s="120" t="s">
         <v>177</v>
       </c>
       <c r="B21" s="44" t="s">
@@ -8066,8 +8137,8 @@
       <c r="I21" s="30"/>
       <c r="J21" s="31"/>
     </row>
-    <row r="22" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A22" s="121"/>
+    <row r="22" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A22" s="120"/>
       <c r="B22" s="44" t="s">
         <v>181</v>
       </c>
@@ -8088,8 +8159,8 @@
       <c r="I22" s="30"/>
       <c r="J22" s="31"/>
     </row>
-    <row r="23" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A23" s="121"/>
+    <row r="23" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A23" s="120"/>
       <c r="B23" s="44" t="s">
         <v>184</v>
       </c>
@@ -8111,7 +8182,7 @@
       <c r="J23" s="31"/>
     </row>
     <row r="24" spans="1:10" s="25" customFormat="1" ht="95.25" customHeight="1">
-      <c r="A24" s="121" t="s">
+      <c r="A24" s="120" t="s">
         <v>187</v>
       </c>
       <c r="B24" s="44" t="s">
@@ -8134,8 +8205,8 @@
       <c r="I24" s="30"/>
       <c r="J24" s="31"/>
     </row>
-    <row r="25" spans="1:10" s="25" customFormat="1" ht="63">
-      <c r="A25" s="121"/>
+    <row r="25" spans="1:10" s="25" customFormat="1" ht="62.4">
+      <c r="A25" s="120"/>
       <c r="B25" s="44" t="s">
         <v>190</v>
       </c>
@@ -8156,8 +8227,8 @@
       <c r="I25" s="30"/>
       <c r="J25" s="31"/>
     </row>
-    <row r="26" spans="1:10" s="25" customFormat="1" ht="63">
-      <c r="A26" s="121"/>
+    <row r="26" spans="1:10" s="25" customFormat="1" ht="62.4">
+      <c r="A26" s="120"/>
       <c r="B26" s="44" t="s">
         <v>192</v>
       </c>
@@ -8178,8 +8249,8 @@
       <c r="I26" s="30"/>
       <c r="J26" s="31"/>
     </row>
-    <row r="27" spans="1:10" s="25" customFormat="1" ht="47.25">
-      <c r="A27" s="121"/>
+    <row r="27" spans="1:10" s="25" customFormat="1" ht="46.8">
+      <c r="A27" s="120"/>
       <c r="B27" s="44" t="s">
         <v>194</v>
       </c>
@@ -8200,8 +8271,8 @@
       <c r="I27" s="30"/>
       <c r="J27" s="31"/>
     </row>
-    <row r="28" spans="1:10" s="25" customFormat="1" ht="110.25">
-      <c r="A28" s="121"/>
+    <row r="28" spans="1:10" s="25" customFormat="1" ht="109.2">
+      <c r="A28" s="120"/>
       <c r="B28" s="44" t="s">
         <v>196</v>
       </c>
@@ -8223,7 +8294,7 @@
       <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" s="25" customFormat="1" ht="48" customHeight="1">
-      <c r="A29" s="121" t="s">
+      <c r="A29" s="120" t="s">
         <v>198</v>
       </c>
       <c r="B29" s="44" t="s">
@@ -8246,8 +8317,8 @@
       <c r="I29" s="28"/>
       <c r="J29" s="32"/>
     </row>
-    <row r="30" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A30" s="121"/>
+    <row r="30" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A30" s="120"/>
       <c r="B30" s="44" t="s">
         <v>201</v>
       </c>
@@ -8268,8 +8339,8 @@
       <c r="I30" s="28"/>
       <c r="J30" s="32"/>
     </row>
-    <row r="31" spans="1:10" s="25" customFormat="1" ht="47.25">
-      <c r="A31" s="121"/>
+    <row r="31" spans="1:10" s="25" customFormat="1" ht="46.8">
+      <c r="A31" s="120"/>
       <c r="B31" s="44" t="s">
         <v>203</v>
       </c>
@@ -8290,8 +8361,8 @@
       <c r="I31" s="28"/>
       <c r="J31" s="32"/>
     </row>
-    <row r="32" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A32" s="121"/>
+    <row r="32" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A32" s="120"/>
       <c r="B32" s="44" t="s">
         <v>205</v>
       </c>
@@ -8312,8 +8383,8 @@
       <c r="I32" s="28"/>
       <c r="J32" s="32"/>
     </row>
-    <row r="33" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A33" s="121"/>
+    <row r="33" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A33" s="120"/>
       <c r="B33" s="44" t="s">
         <v>207</v>
       </c>
@@ -8334,8 +8405,8 @@
       <c r="I33" s="28"/>
       <c r="J33" s="32"/>
     </row>
-    <row r="34" spans="1:10" s="25" customFormat="1" ht="63">
-      <c r="A34" s="121"/>
+    <row r="34" spans="1:10" s="25" customFormat="1" ht="62.4">
+      <c r="A34" s="120"/>
       <c r="B34" s="44" t="s">
         <v>210</v>
       </c>
@@ -8356,8 +8427,8 @@
       <c r="I34" s="28"/>
       <c r="J34" s="32"/>
     </row>
-    <row r="35" spans="1:10" s="25" customFormat="1" ht="47.25">
-      <c r="A35" s="121"/>
+    <row r="35" spans="1:10" s="25" customFormat="1" ht="46.8">
+      <c r="A35" s="120"/>
       <c r="B35" s="44" t="s">
         <v>212</v>
       </c>
@@ -8379,7 +8450,7 @@
       <c r="J35" s="32"/>
     </row>
     <row r="36" spans="1:10" s="25" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A36" s="121" t="s">
+      <c r="A36" s="120" t="s">
         <v>214</v>
       </c>
       <c r="B36" s="44" t="s">
@@ -8402,8 +8473,8 @@
       <c r="I36" s="28"/>
       <c r="J36" s="32"/>
     </row>
-    <row r="37" spans="1:10" s="25" customFormat="1" ht="47.25">
-      <c r="A37" s="121"/>
+    <row r="37" spans="1:10" s="25" customFormat="1" ht="46.8">
+      <c r="A37" s="120"/>
       <c r="B37" s="44" t="s">
         <v>218</v>
       </c>
@@ -8424,8 +8495,8 @@
       <c r="I37" s="28"/>
       <c r="J37" s="32"/>
     </row>
-    <row r="38" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A38" s="121"/>
+    <row r="38" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A38" s="120"/>
       <c r="B38" s="44" t="s">
         <v>220</v>
       </c>
@@ -8447,7 +8518,7 @@
       <c r="J38" s="32"/>
     </row>
     <row r="39" spans="1:10" s="25" customFormat="1" ht="48" customHeight="1">
-      <c r="A39" s="121" t="s">
+      <c r="A39" s="120" t="s">
         <v>222</v>
       </c>
       <c r="B39" s="44" t="s">
@@ -8470,8 +8541,8 @@
       <c r="I39" s="28"/>
       <c r="J39" s="32"/>
     </row>
-    <row r="40" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A40" s="121"/>
+    <row r="40" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A40" s="120"/>
       <c r="B40" s="44" t="s">
         <v>226</v>
       </c>
@@ -8492,8 +8563,8 @@
       <c r="I40" s="28"/>
       <c r="J40" s="32"/>
     </row>
-    <row r="41" spans="1:10" s="25" customFormat="1" ht="47.25">
-      <c r="A41" s="121"/>
+    <row r="41" spans="1:10" s="25" customFormat="1" ht="46.8">
+      <c r="A41" s="120"/>
       <c r="B41" s="44" t="s">
         <v>228</v>
       </c>
@@ -8514,8 +8585,8 @@
       <c r="I41" s="28"/>
       <c r="J41" s="32"/>
     </row>
-    <row r="42" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A42" s="121"/>
+    <row r="42" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A42" s="120"/>
       <c r="B42" s="44" t="s">
         <v>230</v>
       </c>
@@ -8536,8 +8607,8 @@
       <c r="I42" s="28"/>
       <c r="J42" s="32"/>
     </row>
-    <row r="43" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A43" s="121"/>
+    <row r="43" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A43" s="120"/>
       <c r="B43" s="44" t="s">
         <v>232</v>
       </c>
@@ -8558,8 +8629,8 @@
       <c r="I43" s="28"/>
       <c r="J43" s="32"/>
     </row>
-    <row r="44" spans="1:10" s="25" customFormat="1" ht="47.25">
-      <c r="A44" s="121"/>
+    <row r="44" spans="1:10" s="25" customFormat="1" ht="46.8">
+      <c r="A44" s="120"/>
       <c r="B44" s="44" t="s">
         <v>234</v>
       </c>
@@ -8581,7 +8652,7 @@
       <c r="J44" s="32"/>
     </row>
     <row r="45" spans="1:10" s="25" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A45" s="121" t="s">
+      <c r="A45" s="120" t="s">
         <v>236</v>
       </c>
       <c r="B45" s="44" t="s">
@@ -8604,8 +8675,8 @@
       <c r="I45" s="28"/>
       <c r="J45" s="32"/>
     </row>
-    <row r="46" spans="1:10" s="25" customFormat="1" ht="47.25">
-      <c r="A46" s="121"/>
+    <row r="46" spans="1:10" s="25" customFormat="1" ht="46.8">
+      <c r="A46" s="120"/>
       <c r="B46" s="44" t="s">
         <v>240</v>
       </c>
@@ -8626,8 +8697,8 @@
       <c r="I46" s="28"/>
       <c r="J46" s="32"/>
     </row>
-    <row r="47" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A47" s="121"/>
+    <row r="47" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A47" s="120"/>
       <c r="B47" s="44" t="s">
         <v>242</v>
       </c>
@@ -8648,8 +8719,8 @@
       <c r="I47" s="28"/>
       <c r="J47" s="32"/>
     </row>
-    <row r="48" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A48" s="121"/>
+    <row r="48" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A48" s="120"/>
       <c r="B48" s="44" t="s">
         <v>244</v>
       </c>
@@ -8670,8 +8741,8 @@
       <c r="I48" s="28"/>
       <c r="J48" s="32"/>
     </row>
-    <row r="49" spans="1:10" s="25" customFormat="1" ht="47.25">
-      <c r="A49" s="121"/>
+    <row r="49" spans="1:10" s="25" customFormat="1" ht="46.8">
+      <c r="A49" s="120"/>
       <c r="B49" s="44" t="s">
         <v>246</v>
       </c>
@@ -8692,8 +8763,8 @@
       <c r="I49" s="28"/>
       <c r="J49" s="32"/>
     </row>
-    <row r="50" spans="1:10" s="25" customFormat="1" ht="47.25">
-      <c r="A50" s="121"/>
+    <row r="50" spans="1:10" s="25" customFormat="1" ht="46.8">
+      <c r="A50" s="120"/>
       <c r="B50" s="44" t="s">
         <v>249</v>
       </c>
@@ -8714,8 +8785,8 @@
       <c r="I50" s="28"/>
       <c r="J50" s="32"/>
     </row>
-    <row r="51" spans="1:10" s="25" customFormat="1" ht="47.25">
-      <c r="A51" s="121"/>
+    <row r="51" spans="1:10" s="25" customFormat="1" ht="46.8">
+      <c r="A51" s="120"/>
       <c r="B51" s="44" t="s">
         <v>252</v>
       </c>
@@ -8737,7 +8808,7 @@
       <c r="J51" s="32"/>
     </row>
     <row r="52" spans="1:10" s="25" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A52" s="121" t="s">
+      <c r="A52" s="120" t="s">
         <v>255</v>
       </c>
       <c r="B52" s="44" t="s">
@@ -8760,8 +8831,8 @@
       <c r="I52" s="28"/>
       <c r="J52" s="32"/>
     </row>
-    <row r="53" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A53" s="121"/>
+    <row r="53" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A53" s="120"/>
       <c r="B53" s="44" t="s">
         <v>259</v>
       </c>
@@ -8782,8 +8853,8 @@
       <c r="I53" s="28"/>
       <c r="J53" s="32"/>
     </row>
-    <row r="54" spans="1:10" s="25" customFormat="1" ht="31.5">
-      <c r="A54" s="121"/>
+    <row r="54" spans="1:10" s="25" customFormat="1" ht="31.2">
+      <c r="A54" s="120"/>
       <c r="B54" s="44" t="s">
         <v>261</v>
       </c>
@@ -8805,7 +8876,7 @@
       <c r="J54" s="32"/>
     </row>
     <row r="55" spans="1:10" s="25" customFormat="1" ht="79.5" customHeight="1">
-      <c r="A55" s="121" t="s">
+      <c r="A55" s="120" t="s">
         <v>263</v>
       </c>
       <c r="B55" s="44" t="s">
@@ -8828,8 +8899,8 @@
       <c r="I55" s="28"/>
       <c r="J55" s="32"/>
     </row>
-    <row r="56" spans="1:10" s="25" customFormat="1" ht="47.25">
-      <c r="A56" s="121"/>
+    <row r="56" spans="1:10" s="25" customFormat="1" ht="46.8">
+      <c r="A56" s="120"/>
       <c r="B56" s="44" t="s">
         <v>268</v>
       </c>
@@ -8850,8 +8921,8 @@
       <c r="I56" s="28"/>
       <c r="J56" s="32"/>
     </row>
-    <row r="57" spans="1:10" s="25" customFormat="1" ht="47.25">
-      <c r="A57" s="121"/>
+    <row r="57" spans="1:10" s="25" customFormat="1" ht="46.8">
+      <c r="A57" s="120"/>
       <c r="B57" s="44" t="s">
         <v>270</v>
       </c>
@@ -8872,8 +8943,8 @@
       <c r="I57" s="28"/>
       <c r="J57" s="32"/>
     </row>
-    <row r="58" spans="1:10" s="25" customFormat="1" ht="94.5">
-      <c r="A58" s="121"/>
+    <row r="58" spans="1:10" s="25" customFormat="1" ht="93.6">
+      <c r="A58" s="120"/>
       <c r="B58" s="44" t="s">
         <v>272</v>
       </c>
@@ -8894,16 +8965,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="A14:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A29:A35"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A39:A44"/>
     <mergeCell ref="A45:A51"/>
     <mergeCell ref="A52:A54"/>
     <mergeCell ref="A55:A58"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="A14:A20"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="A29:A35"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="G2:G58" xr:uid="{00000000-0002-0000-0200-000000000000}">
@@ -8928,18 +8999,18 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" style="58" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="25" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="59" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="59"/>
+    <col min="1" max="1" width="40.88671875" style="58" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" style="25" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" style="59" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="59"/>
     <col min="6" max="6" width="70" style="25" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" style="25" customWidth="1"/>
-    <col min="8" max="8" width="36.140625" style="25" customWidth="1"/>
-    <col min="9" max="9" width="35.7109375" style="25" customWidth="1"/>
-    <col min="10" max="10" width="42.85546875" style="25" customWidth="1"/>
-    <col min="11" max="1024" width="8.85546875" style="25"/>
+    <col min="7" max="7" width="20.5546875" style="25" customWidth="1"/>
+    <col min="8" max="8" width="36.109375" style="25" customWidth="1"/>
+    <col min="9" max="9" width="35.6640625" style="25" customWidth="1"/>
+    <col min="10" max="10" width="42.88671875" style="25" customWidth="1"/>
+    <col min="11" max="1024" width="8.88671875" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="43" customFormat="1" ht="42">
@@ -8997,7 +9068,7 @@
       <c r="J2" s="65"/>
     </row>
     <row r="3" spans="1:10" ht="63.75" customHeight="1">
-      <c r="A3" s="121" t="s">
+      <c r="A3" s="120" t="s">
         <v>277</v>
       </c>
       <c r="B3" s="62" t="s">
@@ -9020,8 +9091,8 @@
       <c r="I3" s="28"/>
       <c r="J3" s="32"/>
     </row>
-    <row r="4" spans="1:10" ht="47.25">
-      <c r="A4" s="121"/>
+    <row r="4" spans="1:10" ht="46.8">
+      <c r="A4" s="120"/>
       <c r="B4" s="62" t="s">
         <v>280</v>
       </c>
@@ -9042,8 +9113,8 @@
       <c r="I4" s="28"/>
       <c r="J4" s="32"/>
     </row>
-    <row r="5" spans="1:10" ht="47.25">
-      <c r="A5" s="121"/>
+    <row r="5" spans="1:10" ht="46.8">
+      <c r="A5" s="120"/>
       <c r="B5" s="62" t="s">
         <v>282</v>
       </c>
@@ -9064,8 +9135,8 @@
       <c r="I5" s="28"/>
       <c r="J5" s="32"/>
     </row>
-    <row r="6" spans="1:10" ht="63">
-      <c r="A6" s="121"/>
+    <row r="6" spans="1:10" ht="62.4">
+      <c r="A6" s="120"/>
       <c r="B6" s="62" t="s">
         <v>284</v>
       </c>
@@ -9087,7 +9158,7 @@
       <c r="J6" s="32"/>
     </row>
     <row r="7" spans="1:10" ht="79.5" customHeight="1">
-      <c r="A7" s="121" t="s">
+      <c r="A7" s="120" t="s">
         <v>286</v>
       </c>
       <c r="B7" s="62" t="s">
@@ -9110,8 +9181,8 @@
       <c r="I7" s="28"/>
       <c r="J7" s="32"/>
     </row>
-    <row r="8" spans="1:10" ht="110.25">
-      <c r="A8" s="121"/>
+    <row r="8" spans="1:10" ht="109.2">
+      <c r="A8" s="120"/>
       <c r="B8" s="62" t="s">
         <v>289</v>
       </c>
@@ -9132,8 +9203,8 @@
       <c r="I8" s="28"/>
       <c r="J8" s="32"/>
     </row>
-    <row r="9" spans="1:10" ht="63">
-      <c r="A9" s="121"/>
+    <row r="9" spans="1:10" ht="62.4">
+      <c r="A9" s="120"/>
       <c r="B9" s="62" t="s">
         <v>291</v>
       </c>
@@ -9152,8 +9223,8 @@
       <c r="I9" s="28"/>
       <c r="J9" s="32"/>
     </row>
-    <row r="10" spans="1:10" ht="31.5">
-      <c r="A10" s="121"/>
+    <row r="10" spans="1:10" ht="31.2">
+      <c r="A10" s="120"/>
       <c r="B10" s="62" t="s">
         <v>293</v>
       </c>
@@ -9175,7 +9246,7 @@
       <c r="J10" s="32"/>
     </row>
     <row r="11" spans="1:10" ht="48" customHeight="1">
-      <c r="A11" s="121" t="s">
+      <c r="A11" s="120" t="s">
         <v>295</v>
       </c>
       <c r="B11" s="62" t="s">
@@ -9198,8 +9269,8 @@
       <c r="I11" s="28"/>
       <c r="J11" s="32"/>
     </row>
-    <row r="12" spans="1:10" ht="47.25">
-      <c r="A12" s="121"/>
+    <row r="12" spans="1:10" ht="46.8">
+      <c r="A12" s="120"/>
       <c r="B12" s="62" t="s">
         <v>299</v>
       </c>
@@ -9220,8 +9291,8 @@
       <c r="I12" s="28"/>
       <c r="J12" s="32"/>
     </row>
-    <row r="13" spans="1:10" ht="63">
-      <c r="A13" s="121"/>
+    <row r="13" spans="1:10" ht="62.4">
+      <c r="A13" s="120"/>
       <c r="B13" s="62" t="s">
         <v>301</v>
       </c>
@@ -9242,8 +9313,8 @@
       <c r="I13" s="28"/>
       <c r="J13" s="32"/>
     </row>
-    <row r="14" spans="1:10" ht="31.5">
-      <c r="A14" s="121"/>
+    <row r="14" spans="1:10" ht="31.2">
+      <c r="A14" s="120"/>
       <c r="B14" s="62" t="s">
         <v>303</v>
       </c>
@@ -9264,8 +9335,8 @@
       <c r="I14" s="28"/>
       <c r="J14" s="32"/>
     </row>
-    <row r="15" spans="1:10" ht="94.5">
-      <c r="A15" s="121"/>
+    <row r="15" spans="1:10" ht="93.6">
+      <c r="A15" s="120"/>
       <c r="B15" s="62" t="s">
         <v>305</v>
       </c>
@@ -9287,7 +9358,7 @@
       <c r="J15" s="32"/>
     </row>
     <row r="16" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A16" s="121" t="s">
+      <c r="A16" s="120" t="s">
         <v>307</v>
       </c>
       <c r="B16" s="62" t="s">
@@ -9310,8 +9381,8 @@
       <c r="I16" s="28"/>
       <c r="J16" s="32"/>
     </row>
-    <row r="17" spans="1:10" ht="31.5">
-      <c r="A17" s="121"/>
+    <row r="17" spans="1:10" ht="31.2">
+      <c r="A17" s="120"/>
       <c r="B17" s="62" t="s">
         <v>311</v>
       </c>
@@ -9330,8 +9401,8 @@
       <c r="I17" s="28"/>
       <c r="J17" s="32"/>
     </row>
-    <row r="18" spans="1:10" ht="47.25">
-      <c r="A18" s="121"/>
+    <row r="18" spans="1:10" ht="46.8">
+      <c r="A18" s="120"/>
       <c r="B18" s="62" t="s">
         <v>313</v>
       </c>
@@ -9351,7 +9422,7 @@
       <c r="J18" s="32"/>
     </row>
     <row r="19" spans="1:10" ht="63.75" customHeight="1">
-      <c r="A19" s="121" t="s">
+      <c r="A19" s="120" t="s">
         <v>315</v>
       </c>
       <c r="B19" s="62" t="s">
@@ -9374,8 +9445,8 @@
       <c r="I19" s="28"/>
       <c r="J19" s="32"/>
     </row>
-    <row r="20" spans="1:10" ht="47.25">
-      <c r="A20" s="121"/>
+    <row r="20" spans="1:10" ht="46.8">
+      <c r="A20" s="120"/>
       <c r="B20" s="62" t="s">
         <v>319</v>
       </c>
@@ -9396,7 +9467,7 @@
       <c r="I20" s="28"/>
       <c r="J20" s="32"/>
     </row>
-    <row r="21" spans="1:10" ht="47.25">
+    <row r="21" spans="1:10" ht="46.8">
       <c r="A21" s="1" t="s">
         <v>321</v>
       </c>
@@ -9454,25 +9525,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" style="72" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="73" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="59" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="59"/>
-    <col min="6" max="6" width="68.7109375" style="25" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" style="25" customWidth="1"/>
-    <col min="8" max="8" width="32.7109375" style="25" customWidth="1"/>
-    <col min="9" max="9" width="27.28515625" style="25" customWidth="1"/>
-    <col min="10" max="10" width="42.140625" style="25" customWidth="1"/>
-    <col min="11" max="1024" width="8.85546875" style="25"/>
+    <col min="1" max="1" width="38.44140625" style="72" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" style="73" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" style="59" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="59"/>
+    <col min="6" max="6" width="68.6640625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" style="25" customWidth="1"/>
+    <col min="8" max="8" width="32.6640625" style="25" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" style="25" customWidth="1"/>
+    <col min="10" max="10" width="42.109375" style="25" customWidth="1"/>
+    <col min="11" max="1024" width="8.88671875" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="76" customFormat="1" ht="37.5">
+    <row r="1" spans="1:10" s="76" customFormat="1">
       <c r="A1" s="40" t="s">
         <v>20</v>
       </c>
@@ -9505,7 +9576,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="48" customHeight="1">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="120" t="s">
         <v>324</v>
       </c>
       <c r="B2" s="77" t="s">
@@ -9526,8 +9597,8 @@
       <c r="I2" s="49"/>
       <c r="J2" s="65"/>
     </row>
-    <row r="3" spans="1:10" ht="47.25">
-      <c r="A3" s="121"/>
+    <row r="3" spans="1:10" ht="46.8">
+      <c r="A3" s="120"/>
       <c r="B3" s="77" t="s">
         <v>327</v>
       </c>
@@ -9546,8 +9617,8 @@
       <c r="I3" s="28"/>
       <c r="J3" s="32"/>
     </row>
-    <row r="4" spans="1:10" ht="94.5">
-      <c r="A4" s="121"/>
+    <row r="4" spans="1:10" ht="93.6">
+      <c r="A4" s="120"/>
       <c r="B4" s="77" t="s">
         <v>329</v>
       </c>
@@ -9566,8 +9637,8 @@
       <c r="I4" s="28"/>
       <c r="J4" s="32"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75">
-      <c r="A5" s="121"/>
+    <row r="5" spans="1:10" ht="15.6">
+      <c r="A5" s="120"/>
       <c r="B5" s="77" t="s">
         <v>331</v>
       </c>
@@ -9588,8 +9659,8 @@
       <c r="I5" s="28"/>
       <c r="J5" s="32"/>
     </row>
-    <row r="6" spans="1:10" ht="47.25">
-      <c r="A6" s="121"/>
+    <row r="6" spans="1:10" ht="46.8">
+      <c r="A6" s="120"/>
       <c r="B6" s="77" t="s">
         <v>332</v>
       </c>
@@ -9609,7 +9680,7 @@
       <c r="J6" s="32"/>
     </row>
     <row r="7" spans="1:10" ht="79.5" customHeight="1">
-      <c r="A7" s="121" t="s">
+      <c r="A7" s="120" t="s">
         <v>334</v>
       </c>
       <c r="B7" s="77" t="s">
@@ -9630,8 +9701,8 @@
       <c r="I7" s="28"/>
       <c r="J7" s="32"/>
     </row>
-    <row r="8" spans="1:10" ht="47.25">
-      <c r="A8" s="121"/>
+    <row r="8" spans="1:10" ht="46.8">
+      <c r="A8" s="120"/>
       <c r="B8" s="77" t="s">
         <v>337</v>
       </c>
@@ -9651,7 +9722,7 @@
       <c r="J8" s="32"/>
     </row>
     <row r="9" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A9" s="121" t="s">
+      <c r="A9" s="120" t="s">
         <v>339</v>
       </c>
       <c r="B9" s="77" t="s">
@@ -9672,8 +9743,8 @@
       <c r="I9" s="28"/>
       <c r="J9" s="32"/>
     </row>
-    <row r="10" spans="1:10" ht="63">
-      <c r="A10" s="121"/>
+    <row r="10" spans="1:10" ht="62.4">
+      <c r="A10" s="120"/>
       <c r="B10" s="77" t="s">
         <v>342</v>
       </c>
@@ -9692,8 +9763,8 @@
       <c r="I10" s="28"/>
       <c r="J10" s="32"/>
     </row>
-    <row r="11" spans="1:10" ht="63">
-      <c r="A11" s="121"/>
+    <row r="11" spans="1:10" ht="62.4">
+      <c r="A11" s="120"/>
       <c r="B11" s="77" t="s">
         <v>344</v>
       </c>
@@ -9737,24 +9808,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J31" sqref="G28:J31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="53.42578125" style="72" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="25" customWidth="1"/>
-    <col min="3" max="5" width="8.85546875" style="59"/>
-    <col min="6" max="6" width="60.7109375" style="25" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" style="25" customWidth="1"/>
-    <col min="8" max="8" width="41.28515625" style="25" customWidth="1"/>
-    <col min="9" max="9" width="35.28515625" style="25" customWidth="1"/>
-    <col min="10" max="10" width="29" style="25" customWidth="1"/>
-    <col min="11" max="1024" width="8.85546875" style="25"/>
+    <col min="1" max="1" width="53.44140625" style="72" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="25" customWidth="1"/>
+    <col min="3" max="5" width="8.88671875" style="59"/>
+    <col min="6" max="6" width="60.6640625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" style="124" customWidth="1"/>
+    <col min="8" max="8" width="41.33203125" style="124" customWidth="1"/>
+    <col min="9" max="9" width="35.33203125" style="124" customWidth="1"/>
+    <col min="10" max="10" width="29" style="124" customWidth="1"/>
+    <col min="11" max="1024" width="8.88671875" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="43" customFormat="1" ht="42">
+    <row r="1" spans="1:10" s="43" customFormat="1" ht="42.6" thickBot="1">
       <c r="A1" s="40" t="s">
         <v>20</v>
       </c>
@@ -9773,21 +9844,21 @@
       <c r="F1" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="61" t="s">
+      <c r="G1" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="61" t="s">
+      <c r="H1" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="61" t="s">
+      <c r="I1" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="61" t="s">
+      <c r="J1" s="60" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="79.5" customHeight="1">
-      <c r="A2" s="121" t="s">
+    <row r="2" spans="1:10" ht="79.5" customHeight="1" thickBot="1">
+      <c r="A2" s="120" t="s">
         <v>346</v>
       </c>
       <c r="B2" s="62" t="s">
@@ -9803,13 +9874,13 @@
       <c r="F2" s="79" t="s">
         <v>348</v>
       </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="65"/>
-    </row>
-    <row r="3" spans="1:10" ht="94.5">
-      <c r="A3" s="121"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="51"/>
+    </row>
+    <row r="3" spans="1:10" ht="94.2" thickBot="1">
+      <c r="A3" s="120"/>
       <c r="B3" s="62" t="s">
         <v>349</v>
       </c>
@@ -9823,13 +9894,13 @@
       <c r="F3" s="80" t="s">
         <v>350</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="32"/>
-    </row>
-    <row r="4" spans="1:10" ht="78.75">
-      <c r="A4" s="121"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="31"/>
+    </row>
+    <row r="4" spans="1:10" ht="78.599999999999994" thickBot="1">
+      <c r="A4" s="120"/>
       <c r="B4" s="62" t="s">
         <v>351</v>
       </c>
@@ -9843,13 +9914,13 @@
       <c r="F4" s="80" t="s">
         <v>352</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="32"/>
-    </row>
-    <row r="5" spans="1:10" ht="110.25">
-      <c r="A5" s="121"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="31"/>
+    </row>
+    <row r="5" spans="1:10" ht="109.8" thickBot="1">
+      <c r="A5" s="120"/>
       <c r="B5" s="62" t="s">
         <v>353</v>
       </c>
@@ -9863,13 +9934,13 @@
       <c r="F5" s="80" t="s">
         <v>354</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="32"/>
-    </row>
-    <row r="6" spans="1:10" ht="47.25">
-      <c r="A6" s="121"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="31"/>
+    </row>
+    <row r="6" spans="1:10" ht="47.4" thickBot="1">
+      <c r="A6" s="120"/>
       <c r="B6" s="62" t="s">
         <v>355</v>
       </c>
@@ -9883,13 +9954,13 @@
       <c r="F6" s="80" t="s">
         <v>356</v>
       </c>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="32"/>
-    </row>
-    <row r="7" spans="1:10" ht="63.75" customHeight="1">
-      <c r="A7" s="121" t="s">
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="31"/>
+    </row>
+    <row r="7" spans="1:10" ht="63.75" customHeight="1" thickBot="1">
+      <c r="A7" s="120" t="s">
         <v>357</v>
       </c>
       <c r="B7" s="62" t="s">
@@ -9905,13 +9976,21 @@
       <c r="F7" s="80" t="s">
         <v>358</v>
       </c>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="32"/>
-    </row>
-    <row r="8" spans="1:10" ht="31.5">
-      <c r="A8" s="121"/>
+      <c r="G7" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>695</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>705</v>
+      </c>
+      <c r="J7" s="31" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="31.8" thickBot="1">
+      <c r="A8" s="120"/>
       <c r="B8" s="62" t="s">
         <v>359</v>
       </c>
@@ -9925,13 +10004,13 @@
       <c r="F8" s="80" t="s">
         <v>360</v>
       </c>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="32"/>
-    </row>
-    <row r="9" spans="1:10" ht="31.5">
-      <c r="A9" s="121"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="31"/>
+    </row>
+    <row r="9" spans="1:10" ht="47.4" thickBot="1">
+      <c r="A9" s="120"/>
       <c r="B9" s="62" t="s">
         <v>253</v>
       </c>
@@ -9945,13 +10024,21 @@
       <c r="F9" s="80" t="s">
         <v>361</v>
       </c>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="32"/>
-    </row>
-    <row r="10" spans="1:10" ht="63">
-      <c r="A10" s="121"/>
+      <c r="G9" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>695</v>
+      </c>
+      <c r="I9" s="30" t="s">
+        <v>706</v>
+      </c>
+      <c r="J9" s="31" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="63" thickBot="1">
+      <c r="A10" s="120"/>
       <c r="B10" s="62" t="s">
         <v>362</v>
       </c>
@@ -9965,13 +10052,21 @@
       <c r="F10" s="80" t="s">
         <v>363</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="32"/>
-    </row>
-    <row r="11" spans="1:10" ht="47.25">
-      <c r="A11" s="121"/>
+      <c r="G10" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>695</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>707</v>
+      </c>
+      <c r="J10" s="31" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="94.2" thickBot="1">
+      <c r="A11" s="120"/>
       <c r="B11" s="62" t="s">
         <v>166</v>
       </c>
@@ -9985,13 +10080,21 @@
       <c r="F11" s="80" t="s">
         <v>364</v>
       </c>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="32"/>
-    </row>
-    <row r="12" spans="1:10" ht="63">
-      <c r="A12" s="121"/>
+      <c r="G11" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>695</v>
+      </c>
+      <c r="I11" s="30" t="s">
+        <v>696</v>
+      </c>
+      <c r="J11" s="31" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="78.599999999999994" thickBot="1">
+      <c r="A12" s="120"/>
       <c r="B12" s="62" t="s">
         <v>169</v>
       </c>
@@ -10005,13 +10108,21 @@
       <c r="F12" s="80" t="s">
         <v>365</v>
       </c>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="32"/>
-    </row>
-    <row r="13" spans="1:10" ht="63">
-      <c r="A13" s="121"/>
+      <c r="G12" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>698</v>
+      </c>
+      <c r="I12" s="30" t="s">
+        <v>708</v>
+      </c>
+      <c r="J12" s="31" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="63" thickBot="1">
+      <c r="A13" s="120"/>
       <c r="B13" s="62" t="s">
         <v>366</v>
       </c>
@@ -10025,13 +10136,21 @@
       <c r="F13" s="80" t="s">
         <v>367</v>
       </c>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="32"/>
-    </row>
-    <row r="14" spans="1:10" ht="63">
-      <c r="A14" s="121"/>
+      <c r="G13" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="30" t="s">
+        <v>695</v>
+      </c>
+      <c r="I13" s="30" t="s">
+        <v>709</v>
+      </c>
+      <c r="J13" s="31" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="63" thickBot="1">
+      <c r="A14" s="120"/>
       <c r="B14" s="62" t="s">
         <v>172</v>
       </c>
@@ -10045,13 +10164,13 @@
       <c r="F14" s="80" t="s">
         <v>368</v>
       </c>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="32"/>
-    </row>
-    <row r="15" spans="1:10" ht="126.75" customHeight="1">
-      <c r="A15" s="121" t="s">
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="31"/>
+    </row>
+    <row r="15" spans="1:10" ht="126.75" customHeight="1" thickBot="1">
+      <c r="A15" s="120" t="s">
         <v>369</v>
       </c>
       <c r="B15" s="62" t="s">
@@ -10067,13 +10186,13 @@
       <c r="F15" s="80" t="s">
         <v>371</v>
       </c>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="32"/>
-    </row>
-    <row r="16" spans="1:10" ht="78.75">
-      <c r="A16" s="121"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="31"/>
+    </row>
+    <row r="16" spans="1:10" ht="78.599999999999994" thickBot="1">
+      <c r="A16" s="120"/>
       <c r="B16" s="62" t="s">
         <v>372</v>
       </c>
@@ -10087,13 +10206,13 @@
       <c r="F16" s="80" t="s">
         <v>373</v>
       </c>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="32"/>
-    </row>
-    <row r="17" spans="1:10" ht="63">
-      <c r="A17" s="121"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="31"/>
+    </row>
+    <row r="17" spans="1:11" ht="63" thickBot="1">
+      <c r="A17" s="120"/>
       <c r="B17" s="62" t="s">
         <v>374</v>
       </c>
@@ -10107,13 +10226,13 @@
       <c r="F17" s="80" t="s">
         <v>375</v>
       </c>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="32"/>
-    </row>
-    <row r="18" spans="1:10" ht="78.75">
-      <c r="A18" s="121"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="31"/>
+    </row>
+    <row r="18" spans="1:11" ht="78.599999999999994" thickBot="1">
+      <c r="A18" s="120"/>
       <c r="B18" s="62" t="s">
         <v>376</v>
       </c>
@@ -10127,13 +10246,13 @@
       <c r="F18" s="80" t="s">
         <v>377</v>
       </c>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="32"/>
-    </row>
-    <row r="19" spans="1:10" ht="94.5">
-      <c r="A19" s="121"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="31"/>
+    </row>
+    <row r="19" spans="1:11" ht="94.2" thickBot="1">
+      <c r="A19" s="120"/>
       <c r="B19" s="62" t="s">
         <v>378</v>
       </c>
@@ -10147,13 +10266,13 @@
       <c r="F19" s="80" t="s">
         <v>379</v>
       </c>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="32"/>
-    </row>
-    <row r="20" spans="1:10" ht="63">
-      <c r="A20" s="121"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="31"/>
+    </row>
+    <row r="20" spans="1:11" ht="63" thickBot="1">
+      <c r="A20" s="120"/>
       <c r="B20" s="62" t="s">
         <v>380</v>
       </c>
@@ -10167,13 +10286,13 @@
       <c r="F20" s="80" t="s">
         <v>381</v>
       </c>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="32"/>
-    </row>
-    <row r="21" spans="1:10" ht="78.75">
-      <c r="A21" s="121"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="31"/>
+    </row>
+    <row r="21" spans="1:11" ht="78.599999999999994" thickBot="1">
+      <c r="A21" s="120"/>
       <c r="B21" s="62" t="s">
         <v>382</v>
       </c>
@@ -10187,13 +10306,13 @@
       <c r="F21" s="80" t="s">
         <v>383</v>
       </c>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="32"/>
-    </row>
-    <row r="22" spans="1:10" ht="78.75">
-      <c r="A22" s="121"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="31"/>
+    </row>
+    <row r="22" spans="1:11" ht="78.599999999999994" thickBot="1">
+      <c r="A22" s="120"/>
       <c r="B22" s="62" t="s">
         <v>384</v>
       </c>
@@ -10207,13 +10326,13 @@
       <c r="F22" s="80" t="s">
         <v>385</v>
       </c>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="32"/>
-    </row>
-    <row r="23" spans="1:10" ht="31.5">
-      <c r="A23" s="121"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="31"/>
+    </row>
+    <row r="23" spans="1:11" ht="31.8" thickBot="1">
+      <c r="A23" s="120"/>
       <c r="B23" s="62" t="s">
         <v>386</v>
       </c>
@@ -10227,13 +10346,13 @@
       <c r="F23" s="80" t="s">
         <v>387</v>
       </c>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="32"/>
-    </row>
-    <row r="24" spans="1:10" ht="47.25">
-      <c r="A24" s="121"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="31"/>
+    </row>
+    <row r="24" spans="1:11" ht="47.4" thickBot="1">
+      <c r="A24" s="120"/>
       <c r="B24" s="62" t="s">
         <v>388</v>
       </c>
@@ -10247,13 +10366,13 @@
       <c r="F24" s="80" t="s">
         <v>389</v>
       </c>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="32"/>
-    </row>
-    <row r="25" spans="1:10" ht="48" customHeight="1">
-      <c r="A25" s="121" t="s">
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="31"/>
+    </row>
+    <row r="25" spans="1:11" ht="48" customHeight="1" thickBot="1">
+      <c r="A25" s="120" t="s">
         <v>390</v>
       </c>
       <c r="B25" s="62" t="s">
@@ -10269,13 +10388,13 @@
       <c r="F25" s="80" t="s">
         <v>392</v>
       </c>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="32"/>
-    </row>
-    <row r="26" spans="1:10" ht="31.5">
-      <c r="A26" s="121"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="31"/>
+    </row>
+    <row r="26" spans="1:11" ht="31.8" thickBot="1">
+      <c r="A26" s="120"/>
       <c r="B26" s="62" t="s">
         <v>393</v>
       </c>
@@ -10289,13 +10408,13 @@
       <c r="F26" s="80" t="s">
         <v>394</v>
       </c>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="32"/>
-    </row>
-    <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="121"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="31"/>
+    </row>
+    <row r="27" spans="1:11" ht="31.8" thickBot="1">
+      <c r="A27" s="120"/>
       <c r="B27" s="62" t="s">
         <v>395</v>
       </c>
@@ -10309,13 +10428,13 @@
       <c r="F27" s="80" t="s">
         <v>396</v>
       </c>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="32"/>
-    </row>
-    <row r="28" spans="1:10" ht="63.75" customHeight="1">
-      <c r="A28" s="121" t="s">
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="31"/>
+    </row>
+    <row r="28" spans="1:11" ht="94.2" thickBot="1">
+      <c r="A28" s="120" t="s">
         <v>397</v>
       </c>
       <c r="B28" s="62" t="s">
@@ -10331,13 +10450,21 @@
       <c r="F28" s="80" t="s">
         <v>399</v>
       </c>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="32"/>
-    </row>
-    <row r="29" spans="1:10" ht="63">
-      <c r="A29" s="121"/>
+      <c r="G28" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28" s="30" t="s">
+        <v>698</v>
+      </c>
+      <c r="I28" s="30" t="s">
+        <v>699</v>
+      </c>
+      <c r="J28" s="31" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="94.2" thickBot="1">
+      <c r="A29" s="120"/>
       <c r="B29" s="62" t="s">
         <v>400</v>
       </c>
@@ -10351,13 +10478,21 @@
       <c r="F29" s="80" t="s">
         <v>401</v>
       </c>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="32"/>
-    </row>
-    <row r="30" spans="1:10" ht="47.25">
-      <c r="A30" s="121"/>
+      <c r="G29" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="H29" s="30" t="s">
+        <v>695</v>
+      </c>
+      <c r="I29" s="30" t="s">
+        <v>701</v>
+      </c>
+      <c r="J29" s="31" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="109.8" thickBot="1">
+      <c r="A30" s="120"/>
       <c r="B30" s="62" t="s">
         <v>402</v>
       </c>
@@ -10371,13 +10506,22 @@
       <c r="F30" s="80" t="s">
         <v>403</v>
       </c>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="32"/>
-    </row>
-    <row r="31" spans="1:10" ht="47.25">
-      <c r="A31" s="121"/>
+      <c r="G30" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="H30" s="30" t="s">
+        <v>698</v>
+      </c>
+      <c r="I30" s="30" t="s">
+        <v>702</v>
+      </c>
+      <c r="J30" s="31" t="s">
+        <v>700</v>
+      </c>
+      <c r="K30" s="125"/>
+    </row>
+    <row r="31" spans="1:11" ht="109.8" thickBot="1">
+      <c r="A31" s="120"/>
       <c r="B31" s="62" t="s">
         <v>404</v>
       </c>
@@ -10391,10 +10535,18 @@
       <c r="F31" s="81" t="s">
         <v>405</v>
       </c>
-      <c r="G31" s="35"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="35"/>
-      <c r="J31" s="37"/>
+      <c r="G31" s="122" t="s">
+        <v>26</v>
+      </c>
+      <c r="H31" s="122" t="s">
+        <v>703</v>
+      </c>
+      <c r="I31" s="122" t="s">
+        <v>704</v>
+      </c>
+      <c r="J31" s="123" t="s">
+        <v>697</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -10411,7 +10563,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -10423,22 +10575,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AMJ17"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" style="72" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="25" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="59" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="59"/>
-    <col min="6" max="6" width="97.140625" style="25" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" style="25" customWidth="1"/>
-    <col min="8" max="8" width="36.140625" style="25" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" style="72" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" style="59" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="59"/>
+    <col min="6" max="6" width="97.109375" style="25" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" style="25" customWidth="1"/>
+    <col min="8" max="8" width="36.109375" style="25" customWidth="1"/>
     <col min="9" max="9" width="18" style="25" customWidth="1"/>
-    <col min="10" max="10" width="27.28515625" style="25" customWidth="1"/>
-    <col min="11" max="1024" width="8.85546875" style="25"/>
+    <col min="10" max="10" width="27.33203125" style="25" customWidth="1"/>
+    <col min="11" max="1024" width="8.88671875" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="43" customFormat="1" ht="42">
@@ -10474,7 +10626,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="48" customHeight="1">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="120" t="s">
         <v>406</v>
       </c>
       <c r="B2" s="62" t="s">
@@ -10495,8 +10647,8 @@
       <c r="I2" s="49"/>
       <c r="J2" s="65"/>
     </row>
-    <row r="3" spans="1:10" ht="31.5">
-      <c r="A3" s="121"/>
+    <row r="3" spans="1:10" ht="31.2">
+      <c r="A3" s="120"/>
       <c r="B3" s="62" t="s">
         <v>409</v>
       </c>
@@ -10515,8 +10667,8 @@
       <c r="I3" s="28"/>
       <c r="J3" s="32"/>
     </row>
-    <row r="4" spans="1:10" ht="47.25">
-      <c r="A4" s="121"/>
+    <row r="4" spans="1:10" ht="46.8">
+      <c r="A4" s="120"/>
       <c r="B4" s="62" t="s">
         <v>182</v>
       </c>
@@ -10536,7 +10688,7 @@
       <c r="J4" s="32"/>
     </row>
     <row r="5" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A5" s="121" t="s">
+      <c r="A5" s="120" t="s">
         <v>412</v>
       </c>
       <c r="B5" s="62" t="s">
@@ -10557,8 +10709,8 @@
       <c r="I5" s="28"/>
       <c r="J5" s="32"/>
     </row>
-    <row r="6" spans="1:10" ht="47.25">
-      <c r="A6" s="121"/>
+    <row r="6" spans="1:10" ht="46.8">
+      <c r="A6" s="120"/>
       <c r="B6" s="62" t="s">
         <v>415</v>
       </c>
@@ -10577,8 +10729,8 @@
       <c r="I6" s="28"/>
       <c r="J6" s="32"/>
     </row>
-    <row r="7" spans="1:10" ht="31.5">
-      <c r="A7" s="121"/>
+    <row r="7" spans="1:10" ht="31.2">
+      <c r="A7" s="120"/>
       <c r="B7" s="62" t="s">
         <v>417</v>
       </c>
@@ -10597,8 +10749,8 @@
       <c r="I7" s="28"/>
       <c r="J7" s="32"/>
     </row>
-    <row r="8" spans="1:10" ht="47.25">
-      <c r="A8" s="121"/>
+    <row r="8" spans="1:10" ht="46.8">
+      <c r="A8" s="120"/>
       <c r="B8" s="62" t="s">
         <v>419</v>
       </c>
@@ -10617,8 +10769,8 @@
       <c r="I8" s="28"/>
       <c r="J8" s="32"/>
     </row>
-    <row r="9" spans="1:10" ht="47.25">
-      <c r="A9" s="121"/>
+    <row r="9" spans="1:10" ht="46.8">
+      <c r="A9" s="120"/>
       <c r="B9" s="62" t="s">
         <v>421</v>
       </c>
@@ -10637,8 +10789,8 @@
       <c r="I9" s="28"/>
       <c r="J9" s="32"/>
     </row>
-    <row r="10" spans="1:10" ht="47.25">
-      <c r="A10" s="121"/>
+    <row r="10" spans="1:10" ht="46.8">
+      <c r="A10" s="120"/>
       <c r="B10" s="62" t="s">
         <v>423</v>
       </c>
@@ -10657,8 +10809,8 @@
       <c r="I10" s="28"/>
       <c r="J10" s="32"/>
     </row>
-    <row r="11" spans="1:10" ht="31.5">
-      <c r="A11" s="121"/>
+    <row r="11" spans="1:10" ht="31.2">
+      <c r="A11" s="120"/>
       <c r="B11" s="62" t="s">
         <v>425</v>
       </c>
@@ -10677,8 +10829,8 @@
       <c r="I11" s="28"/>
       <c r="J11" s="32"/>
     </row>
-    <row r="12" spans="1:10" ht="31.5">
-      <c r="A12" s="121"/>
+    <row r="12" spans="1:10" ht="31.2">
+      <c r="A12" s="120"/>
       <c r="B12" s="62" t="s">
         <v>427</v>
       </c>
@@ -10698,7 +10850,7 @@
       <c r="J12" s="32"/>
     </row>
     <row r="13" spans="1:10" ht="48" customHeight="1">
-      <c r="A13" s="121" t="s">
+      <c r="A13" s="120" t="s">
         <v>429</v>
       </c>
       <c r="B13" s="62" t="s">
@@ -10719,8 +10871,8 @@
       <c r="I13" s="28"/>
       <c r="J13" s="32"/>
     </row>
-    <row r="14" spans="1:10" ht="47.25">
-      <c r="A14" s="121"/>
+    <row r="14" spans="1:10" ht="46.8">
+      <c r="A14" s="120"/>
       <c r="B14" s="62" t="s">
         <v>432</v>
       </c>
@@ -10739,8 +10891,8 @@
       <c r="I14" s="28"/>
       <c r="J14" s="32"/>
     </row>
-    <row r="15" spans="1:10" ht="31.5">
-      <c r="A15" s="121"/>
+    <row r="15" spans="1:10" ht="31.2">
+      <c r="A15" s="120"/>
       <c r="B15" s="62" t="s">
         <v>434</v>
       </c>
@@ -10760,7 +10912,7 @@
       <c r="J15" s="32"/>
     </row>
     <row r="16" spans="1:10" ht="48" customHeight="1">
-      <c r="A16" s="121" t="s">
+      <c r="A16" s="120" t="s">
         <v>436</v>
       </c>
       <c r="B16" s="62" t="s">
@@ -10781,8 +10933,8 @@
       <c r="I16" s="28"/>
       <c r="J16" s="32"/>
     </row>
-    <row r="17" spans="1:10" ht="47.25">
-      <c r="A17" s="121"/>
+    <row r="17" spans="1:10" ht="46.8">
+      <c r="A17" s="120"/>
       <c r="B17" s="62" t="s">
         <v>439</v>
       </c>
@@ -10827,25 +10979,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AMJ14"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" style="72" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" style="25" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="59" customWidth="1"/>
-    <col min="4" max="5" width="8.85546875" style="59"/>
-    <col min="6" max="6" width="80.28515625" style="25" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="25" customWidth="1"/>
-    <col min="8" max="8" width="31" style="25" customWidth="1"/>
-    <col min="9" max="9" width="24" style="25" customWidth="1"/>
-    <col min="10" max="10" width="35.140625" style="25" customWidth="1"/>
-    <col min="11" max="1024" width="8.85546875" style="25"/>
+    <col min="1" max="1" width="31.5546875" style="72" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" style="59" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" style="59"/>
+    <col min="6" max="6" width="80.33203125" style="25" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="25" customWidth="1"/>
+    <col min="8" max="8" width="31" style="124" customWidth="1"/>
+    <col min="9" max="9" width="32.88671875" style="124" customWidth="1"/>
+    <col min="10" max="10" width="35.109375" style="124" customWidth="1"/>
+    <col min="11" max="1024" width="8.88671875" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="87" customFormat="1">
+    <row r="1" spans="1:10" s="87" customFormat="1" ht="21.6" thickBot="1">
       <c r="A1" s="83" t="s">
         <v>20</v>
       </c>
@@ -10867,18 +11019,18 @@
       <c r="G1" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="86" t="s">
+      <c r="H1" s="85" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="86" t="s">
+      <c r="I1" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="86" t="s">
+      <c r="J1" s="85" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="48" customHeight="1">
-      <c r="A2" s="121" t="s">
+    <row r="2" spans="1:10" ht="48" customHeight="1" thickBot="1">
+      <c r="A2" s="120" t="s">
         <v>441</v>
       </c>
       <c r="B2" s="62" t="s">
@@ -10895,12 +11047,12 @@
         <v>442</v>
       </c>
       <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="93"/>
-    </row>
-    <row r="3" spans="1:10" ht="47.25">
-      <c r="A3" s="121"/>
+      <c r="H2" s="126"/>
+      <c r="I2" s="126"/>
+      <c r="J2" s="127"/>
+    </row>
+    <row r="3" spans="1:10" ht="47.4" thickBot="1">
+      <c r="A3" s="120"/>
       <c r="B3" s="62" t="s">
         <v>309</v>
       </c>
@@ -10915,12 +11067,12 @@
         <v>443</v>
       </c>
       <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="32"/>
-    </row>
-    <row r="4" spans="1:10" ht="63">
-      <c r="A4" s="121"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="31"/>
+    </row>
+    <row r="4" spans="1:10" ht="63" thickBot="1">
+      <c r="A4" s="120"/>
       <c r="B4" s="62" t="s">
         <v>444</v>
       </c>
@@ -10935,12 +11087,12 @@
         <v>445</v>
       </c>
       <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="32"/>
-    </row>
-    <row r="5" spans="1:10" ht="47.25">
-      <c r="A5" s="121"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="31"/>
+    </row>
+    <row r="5" spans="1:10" ht="47.4" thickBot="1">
+      <c r="A5" s="120"/>
       <c r="B5" s="62" t="s">
         <v>446</v>
       </c>
@@ -10955,12 +11107,12 @@
         <v>447</v>
       </c>
       <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="32"/>
-    </row>
-    <row r="6" spans="1:10" ht="48" customHeight="1">
-      <c r="A6" s="121" t="s">
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="31"/>
+    </row>
+    <row r="6" spans="1:10" ht="48" customHeight="1" thickBot="1">
+      <c r="A6" s="120" t="s">
         <v>448</v>
       </c>
       <c r="B6" s="62" t="s">
@@ -10977,12 +11129,12 @@
         <v>449</v>
       </c>
       <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="32"/>
-    </row>
-    <row r="7" spans="1:10" ht="47.25">
-      <c r="A7" s="121"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="31"/>
+    </row>
+    <row r="7" spans="1:10" ht="47.4" thickBot="1">
+      <c r="A7" s="120"/>
       <c r="B7" s="62" t="s">
         <v>450</v>
       </c>
@@ -10997,12 +11149,12 @@
         <v>451</v>
       </c>
       <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="32"/>
-    </row>
-    <row r="8" spans="1:10" ht="48" customHeight="1">
-      <c r="A8" s="121" t="s">
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="31"/>
+    </row>
+    <row r="8" spans="1:10" ht="48" customHeight="1" thickBot="1">
+      <c r="A8" s="120" t="s">
         <v>452</v>
       </c>
       <c r="B8" s="62" t="s">
@@ -11019,12 +11171,12 @@
         <v>454</v>
       </c>
       <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="32"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75">
-      <c r="A9" s="121"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="31"/>
+    </row>
+    <row r="9" spans="1:10" ht="16.2" thickBot="1">
+      <c r="A9" s="120"/>
       <c r="B9" s="62" t="s">
         <v>455</v>
       </c>
@@ -11041,12 +11193,12 @@
       <c r="G9" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="32"/>
-    </row>
-    <row r="10" spans="1:10" ht="31.5">
-      <c r="A10" s="121"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="31"/>
+    </row>
+    <row r="10" spans="1:10" ht="31.8" thickBot="1">
+      <c r="A10" s="120"/>
       <c r="B10" s="62" t="s">
         <v>457</v>
       </c>
@@ -11061,12 +11213,12 @@
         <v>458</v>
       </c>
       <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="32"/>
-    </row>
-    <row r="11" spans="1:10" ht="63">
-      <c r="A11" s="121"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="31"/>
+    </row>
+    <row r="11" spans="1:10" ht="63" thickBot="1">
+      <c r="A11" s="120"/>
       <c r="B11" s="62" t="s">
         <v>459</v>
       </c>
@@ -11079,12 +11231,12 @@
         <v>460</v>
       </c>
       <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="32"/>
-    </row>
-    <row r="12" spans="1:10" ht="63.75" customHeight="1">
-      <c r="A12" s="121" t="s">
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="31"/>
+    </row>
+    <row r="12" spans="1:10" ht="125.4" thickBot="1">
+      <c r="A12" s="120" t="s">
         <v>461</v>
       </c>
       <c r="B12" s="62" t="s">
@@ -11100,13 +11252,21 @@
       <c r="F12" s="80" t="s">
         <v>463</v>
       </c>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="32"/>
-    </row>
-    <row r="13" spans="1:10" ht="47.25">
-      <c r="A13" s="121"/>
+      <c r="G12" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>698</v>
+      </c>
+      <c r="I12" s="30" t="s">
+        <v>710</v>
+      </c>
+      <c r="J12" s="31" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="47.4" thickBot="1">
+      <c r="A13" s="120"/>
       <c r="B13" s="62" t="s">
         <v>464</v>
       </c>
@@ -11121,12 +11281,12 @@
         <v>465</v>
       </c>
       <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="32"/>
-    </row>
-    <row r="14" spans="1:10" ht="47.25">
-      <c r="A14" s="121"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="31"/>
+    </row>
+    <row r="14" spans="1:10" ht="47.4" thickBot="1">
+      <c r="A14" s="120"/>
       <c r="B14" s="62" t="s">
         <v>466</v>
       </c>
@@ -11141,9 +11301,9 @@
         <v>467</v>
       </c>
       <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="37"/>
+      <c r="H14" s="122"/>
+      <c r="I14" s="122"/>
+      <c r="J14" s="123"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -11175,21 +11335,21 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="72" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="25"/>
-    <col min="3" max="5" width="8.85546875" style="59"/>
+    <col min="1" max="1" width="30.6640625" style="72" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="25"/>
+    <col min="3" max="5" width="8.88671875" style="59"/>
     <col min="6" max="6" width="93" style="25" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="25" customWidth="1"/>
-    <col min="8" max="8" width="35.85546875" style="25" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="25" customWidth="1"/>
-    <col min="10" max="10" width="30.85546875" style="25" customWidth="1"/>
-    <col min="11" max="1024" width="8.85546875" style="25"/>
+    <col min="7" max="7" width="12.44140625" style="25" customWidth="1"/>
+    <col min="8" max="8" width="35.88671875" style="25" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" style="25" customWidth="1"/>
+    <col min="10" max="10" width="30.88671875" style="25" customWidth="1"/>
+    <col min="11" max="1024" width="8.88671875" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="43" customFormat="1" ht="42">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="93" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="61" t="s">
@@ -11221,7 +11381,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="120" t="s">
         <v>468</v>
       </c>
       <c r="B2" s="62" t="s">
@@ -11242,8 +11402,8 @@
       <c r="I2" s="49"/>
       <c r="J2" s="65"/>
     </row>
-    <row r="3" spans="1:10" ht="47.25">
-      <c r="A3" s="121"/>
+    <row r="3" spans="1:10" ht="46.8">
+      <c r="A3" s="120"/>
       <c r="B3" s="62" t="s">
         <v>471</v>
       </c>
@@ -11262,8 +11422,8 @@
       <c r="I3" s="28"/>
       <c r="J3" s="32"/>
     </row>
-    <row r="4" spans="1:10" ht="31.5">
-      <c r="A4" s="121"/>
+    <row r="4" spans="1:10" ht="31.2">
+      <c r="A4" s="120"/>
       <c r="B4" s="62" t="s">
         <v>473</v>
       </c>
@@ -11282,8 +11442,8 @@
       <c r="I4" s="28"/>
       <c r="J4" s="32"/>
     </row>
-    <row r="5" spans="1:10" ht="31.5">
-      <c r="A5" s="121"/>
+    <row r="5" spans="1:10" ht="31.2">
+      <c r="A5" s="120"/>
       <c r="B5" s="62" t="s">
         <v>475</v>
       </c>
@@ -11302,8 +11462,8 @@
       <c r="I5" s="28"/>
       <c r="J5" s="32"/>
     </row>
-    <row r="6" spans="1:10" ht="31.5">
-      <c r="A6" s="121"/>
+    <row r="6" spans="1:10" ht="31.2">
+      <c r="A6" s="120"/>
       <c r="B6" s="62" t="s">
         <v>477</v>
       </c>
@@ -11322,8 +11482,8 @@
       <c r="I6" s="28"/>
       <c r="J6" s="32"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75">
-      <c r="A7" s="121"/>
+    <row r="7" spans="1:10" ht="15.6">
+      <c r="A7" s="120"/>
       <c r="B7" s="62" t="s">
         <v>479</v>
       </c>
@@ -11343,7 +11503,7 @@
       <c r="J7" s="32"/>
     </row>
     <row r="8" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A8" s="121" t="s">
+      <c r="A8" s="120" t="s">
         <v>481</v>
       </c>
       <c r="B8" s="62" t="s">
@@ -11364,8 +11524,8 @@
       <c r="I8" s="28"/>
       <c r="J8" s="32"/>
     </row>
-    <row r="9" spans="1:10" ht="31.5">
-      <c r="A9" s="121"/>
+    <row r="9" spans="1:10" ht="31.2">
+      <c r="A9" s="120"/>
       <c r="B9" s="62" t="s">
         <v>484</v>
       </c>
@@ -11384,8 +11544,8 @@
       <c r="I9" s="28"/>
       <c r="J9" s="32"/>
     </row>
-    <row r="10" spans="1:10" ht="31.5">
-      <c r="A10" s="121"/>
+    <row r="10" spans="1:10" ht="31.2">
+      <c r="A10" s="120"/>
       <c r="B10" s="62" t="s">
         <v>486</v>
       </c>
@@ -11405,7 +11565,7 @@
       <c r="J10" s="32"/>
     </row>
     <row r="11" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A11" s="121" t="s">
+      <c r="A11" s="120" t="s">
         <v>488</v>
       </c>
       <c r="B11" s="62" t="s">
@@ -11426,8 +11586,8 @@
       <c r="I11" s="28"/>
       <c r="J11" s="32"/>
     </row>
-    <row r="12" spans="1:10" ht="15.75">
-      <c r="A12" s="121"/>
+    <row r="12" spans="1:10" ht="15.6">
+      <c r="A12" s="120"/>
       <c r="B12" s="62" t="s">
         <v>491</v>
       </c>
@@ -11446,8 +11606,8 @@
       <c r="I12" s="28"/>
       <c r="J12" s="32"/>
     </row>
-    <row r="13" spans="1:10" ht="47.25">
-      <c r="A13" s="121"/>
+    <row r="13" spans="1:10" ht="46.8">
+      <c r="A13" s="120"/>
       <c r="B13" s="62" t="s">
         <v>493</v>
       </c>
@@ -11466,8 +11626,8 @@
       <c r="I13" s="28"/>
       <c r="J13" s="32"/>
     </row>
-    <row r="14" spans="1:10" ht="47.25">
-      <c r="A14" s="121"/>
+    <row r="14" spans="1:10" ht="46.8">
+      <c r="A14" s="120"/>
       <c r="B14" s="62" t="s">
         <v>495</v>
       </c>
@@ -11486,8 +11646,8 @@
       <c r="I14" s="28"/>
       <c r="J14" s="32"/>
     </row>
-    <row r="15" spans="1:10" ht="31.5">
-      <c r="A15" s="121"/>
+    <row r="15" spans="1:10" ht="31.2">
+      <c r="A15" s="120"/>
       <c r="B15" s="62" t="s">
         <v>497</v>
       </c>
@@ -11506,8 +11666,8 @@
       <c r="I15" s="28"/>
       <c r="J15" s="32"/>
     </row>
-    <row r="16" spans="1:10" ht="31.5">
-      <c r="A16" s="121"/>
+    <row r="16" spans="1:10" ht="31.2">
+      <c r="A16" s="120"/>
       <c r="B16" s="62" t="s">
         <v>499</v>
       </c>
@@ -11526,8 +11686,8 @@
       <c r="I16" s="28"/>
       <c r="J16" s="32"/>
     </row>
-    <row r="17" spans="1:10" ht="47.25">
-      <c r="A17" s="121"/>
+    <row r="17" spans="1:10" ht="46.8">
+      <c r="A17" s="120"/>
       <c r="B17" s="62" t="s">
         <v>501</v>
       </c>
@@ -11546,8 +11706,8 @@
       <c r="I17" s="28"/>
       <c r="J17" s="32"/>
     </row>
-    <row r="18" spans="1:10" ht="31.5">
-      <c r="A18" s="121"/>
+    <row r="18" spans="1:10" ht="31.2">
+      <c r="A18" s="120"/>
       <c r="B18" s="62" t="s">
         <v>503</v>
       </c>
@@ -11588,6 +11748,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="caec8013-4252-46d5-9263-a99cc59dead2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d77a0e16-36e2-4619-a824-6737dea303d4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E2F6ACCA1C4E9E429EC0979D7AA69E5C" ma:contentTypeVersion="14" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="2bb008ca7a1b4eda16785ddef8185b41">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="caec8013-4252-46d5-9263-a99cc59dead2" xmlns:ns3="d77a0e16-36e2-4619-a824-6737dea303d4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a3d1966398a198bcd33f0542821d602e" ns2:_="" ns3:_="">
     <xsd:import namespace="caec8013-4252-46d5-9263-a99cc59dead2"/>
@@ -11816,17 +11987,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="caec8013-4252-46d5-9263-a99cc59dead2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d77a0e16-36e2-4619-a824-6737dea303d4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -11837,6 +11997,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB94848C-75E5-4594-8307-209BB5BE433B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d77a0e16-36e2-4619-a824-6737dea303d4"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="caec8013-4252-46d5-9263-a99cc59dead2"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{088014DA-7408-4969-8EBB-5375B357E254}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11855,23 +12032,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB94848C-75E5-4594-8307-209BB5BE433B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d77a0e16-36e2-4619-a824-6737dea303d4"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="caec8013-4252-46d5-9263-a99cc59dead2"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1115CF8-E078-4757-AB4D-549A55AF833E}">
   <ds:schemaRefs>

</xml_diff>